<commit_message>
Actualización - Arreglo de formulas
</commit_message>
<xml_diff>
--- a/Tarea_1_Analisis_Algoritmos_Emmanuel_Rosales.xlsx
+++ b/Tarea_1_Analisis_Algoritmos_Emmanuel_Rosales.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-460" windowWidth="28800" windowHeight="18000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Configuración 1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="14">
   <si>
     <t>Tarea número 1 -Análisis de algoritmos - Emmanuel Rosales Salas - 2013108931</t>
   </si>
@@ -75,7 +75,7 @@
     <numFmt numFmtId="164" formatCode="#,##0.00;[Red]#,##0.00"/>
     <numFmt numFmtId="165" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
   </numFmts>
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -163,13 +163,6 @@
       <family val="2"/>
     </font>
     <font>
-      <b/>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -243,7 +236,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="15">
+  <cellStyleXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -259,8 +252,24 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -313,28 +322,19 @@
     <xf numFmtId="37" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="37" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="37" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="37" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="39" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -342,12 +342,6 @@
     </xf>
     <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="39" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="39" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -361,8 +355,11 @@
     <xf numFmtId="4" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="37" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="15">
+  <cellStyles count="31">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -370,6 +367,14 @@
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -377,6 +382,14 @@
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -408,7 +421,17 @@
   <c:chart>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.117900553174524"/>
+          <c:y val="0.0166435506241331"/>
+          <c:w val="0.701509643177514"/>
+          <c:h val="0.893629364290629"/>
+        </c:manualLayout>
+      </c:layout>
       <c:lineChart>
         <c:grouping val="stacked"/>
         <c:varyColors val="0"/>
@@ -532,94 +555,94 @@
                 <c:formatCode>#,##0;\-#,##0</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>2.2306002E7</c:v>
+                  <c:v>2.3583429E7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8.9112002E7</c:v>
+                  <c:v>9.4166929E7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.00418002E8</c:v>
+                  <c:v>2.11750429E8</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.56224002E8</c:v>
+                  <c:v>3.76333929E8</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.56530002E8</c:v>
+                  <c:v>5.87917429E8</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8.01336002E8</c:v>
+                  <c:v>8.46500929E8</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.090642002E9</c:v>
+                  <c:v>1.152084429E9</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.424448002E9</c:v>
+                  <c:v>1.504667929E9</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.802754002E9</c:v>
+                  <c:v>1.904251429E9</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.225560002E9</c:v>
+                  <c:v>2.350834929E9</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.692866002E9</c:v>
+                  <c:v>2.844418429E9</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3.204672002E9</c:v>
+                  <c:v>3.385001929E9</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3.760978002E9</c:v>
+                  <c:v>3.972585429E9</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>4.361784002E9</c:v>
+                  <c:v>4.607168929E9</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>5.007090002E9</c:v>
+                  <c:v>5.288752429E9</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>5.696896002E9</c:v>
+                  <c:v>6.017335929E9</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>6.431202002E9</c:v>
+                  <c:v>6.792919429E9</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>7.210008002E9</c:v>
+                  <c:v>7.615502929E9</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>8.033314002E9</c:v>
+                  <c:v>8.485086429E9</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>8.901120002E9</c:v>
+                  <c:v>9.401669929E9</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>9.813426002E9</c:v>
+                  <c:v>1.0365253429E10</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1.0770232002E10</c:v>
+                  <c:v>1.1375836929E10</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>1.1771538002E10</c:v>
+                  <c:v>1.2433420429E10</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>1.2817344002E10</c:v>
+                  <c:v>1.3538003929E10</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>1.3907650002E10</c:v>
+                  <c:v>1.4689587429E10</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>1.5042456002E10</c:v>
+                  <c:v>1.5888170929E10</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>1.6221762002E10</c:v>
+                  <c:v>1.7133754429E10</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>1.7445568002E10</c:v>
+                  <c:v>1.8426337929E10</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>1.8713874002E10</c:v>
+                  <c:v>1.9765921429E10</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>2.0026680002E10</c:v>
+                  <c:v>2.1152504929E10</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -746,94 +769,94 @@
                 <c:formatCode>#,##0;\-#,##0</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>1.3817502E7</c:v>
+                  <c:v>1.4231096E7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.5135002E7</c:v>
+                  <c:v>5.6712346E7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.23952502E8</c:v>
+                  <c:v>1.27443596E8</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.20270002E8</c:v>
+                  <c:v>2.26424846E8</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.44087502E8</c:v>
+                  <c:v>3.53656096E8</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.95405002E8</c:v>
+                  <c:v>5.09137346E8</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6.74222502E8</c:v>
+                  <c:v>6.92868596E8</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8.80540002E8</c:v>
+                  <c:v>9.04849846E8</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.114357502E9</c:v>
+                  <c:v>1.145081096E9</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.375675002E9</c:v>
+                  <c:v>1.413562346E9</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.664492502E9</c:v>
+                  <c:v>1.710293596E9</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.980810002E9</c:v>
+                  <c:v>2.035274846E9</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2.324627502E9</c:v>
+                  <c:v>2.388506096E9</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2.695945002E9</c:v>
+                  <c:v>2.769987346E9</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3.094762502E9</c:v>
+                  <c:v>3.179718596E9</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>3.521080002E9</c:v>
+                  <c:v>3.617699846E9</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>3.974897502E9</c:v>
+                  <c:v>4.083931096E9</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>4.456215002E9</c:v>
+                  <c:v>4.578412346E9</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>4.965032502E9</c:v>
+                  <c:v>5.101143596E9</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>5.501350002E9</c:v>
+                  <c:v>5.652124846E9</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>6.065167502E9</c:v>
+                  <c:v>6.231356096E9</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>6.656485002E9</c:v>
+                  <c:v>6.838837346E9</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>7.275302502E9</c:v>
+                  <c:v>7.474568596E9</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>7.921620002E9</c:v>
+                  <c:v>8.138549846E9</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>8.595437502E9</c:v>
+                  <c:v>8.830781096E9</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>9.296755002E9</c:v>
+                  <c:v>9.551262346E9</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>1.0025572502E10</c:v>
+                  <c:v>1.0299993596E10</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>1.0781890002E10</c:v>
+                  <c:v>1.1076974846E10</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>1.1565707502E10</c:v>
+                  <c:v>1.1882206096E10</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>1.2377025002E10</c:v>
+                  <c:v>1.2715687346E10</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -850,11 +873,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2147426088"/>
-        <c:axId val="-2147433656"/>
+        <c:axId val="-2122585272"/>
+        <c:axId val="-2120281896"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2147426088"/>
+        <c:axId val="-2122585272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -864,7 +887,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2147433656"/>
+        <c:crossAx val="-2120281896"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -872,7 +895,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2147433656"/>
+        <c:axId val="-2120281896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -883,7 +906,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2147426088"/>
+        <c:crossAx val="-2122585272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1045,94 +1068,94 @@
                 <c:formatCode>#,##0;\-#,##0</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>2.2003700005E10</c:v>
+                  <c:v>2.3583429E7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.4258885005E10</c:v>
+                  <c:v>9.4166929E7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.6624070005E10</c:v>
+                  <c:v>2.11750429E8</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.9099255005E10</c:v>
+                  <c:v>3.76333929E8</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.4379625005E10</c:v>
+                  <c:v>5.87917429E8</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.7184810005E10</c:v>
+                  <c:v>8.46500929E8</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4.0099995005E10</c:v>
+                  <c:v>1.152084429E9</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4.3125180005E10</c:v>
+                  <c:v>1.504667929E9</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4.6260365005E10</c:v>
+                  <c:v>1.904251429E9</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4.9505550005E10</c:v>
+                  <c:v>2.350834929E9</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5.2860735005E10</c:v>
+                  <c:v>2.844418429E9</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>5.6325920005E10</c:v>
+                  <c:v>3.385001929E9</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>5.9901105005E10</c:v>
+                  <c:v>3.972585429E9</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>6.3586290005E10</c:v>
+                  <c:v>4.607168929E9</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>6.7381475005E10</c:v>
+                  <c:v>5.288752429E9</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>7.1286660005E10</c:v>
+                  <c:v>6.017335929E9</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>7.5301845005E10</c:v>
+                  <c:v>6.792919429E9</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>7.9427030005E10</c:v>
+                  <c:v>7.615502929E9</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>8.3662215005E10</c:v>
+                  <c:v>8.485086429E9</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>8.8007400005E10</c:v>
+                  <c:v>9.401669929E9</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>9.2462585005E10</c:v>
+                  <c:v>1.0365253429E10</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>9.7027770005E10</c:v>
+                  <c:v>1.1375836929E10</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>1.01702955005E11</c:v>
+                  <c:v>1.2433420429E10</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>1.06488140005E11</c:v>
+                  <c:v>1.3538003929E10</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>1.11383325005E11</c:v>
+                  <c:v>1.4689587429E10</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>1.16388510005E11</c:v>
+                  <c:v>1.5888170929E10</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>1.21503695005E11</c:v>
+                  <c:v>1.7133754429E10</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>1.26728880005E11</c:v>
+                  <c:v>1.8426337929E10</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>1.32064065005E11</c:v>
+                  <c:v>1.9765921429E10</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>1.37509250005E11</c:v>
+                  <c:v>2.1152504929E10</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1259,94 +1282,94 @@
                 <c:formatCode>#,##0;\-#,##0</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>1.7504650005E10</c:v>
+                  <c:v>1.4231096E7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.9298632505E10</c:v>
+                  <c:v>5.6712346E7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.1180115005E10</c:v>
+                  <c:v>1.27443596E8</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.3149097505E10</c:v>
+                  <c:v>2.26424846E8</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.7349562505E10</c:v>
+                  <c:v>3.53656096E8</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.9581045005E10</c:v>
+                  <c:v>5.09137346E8</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.1900027505E10</c:v>
+                  <c:v>6.92868596E8</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.4306510005E10</c:v>
+                  <c:v>9.04849846E8</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.6800492505E10</c:v>
+                  <c:v>1.145081096E9</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3.9381975005E10</c:v>
+                  <c:v>1.413562346E9</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>4.2050957505E10</c:v>
+                  <c:v>1.710293596E9</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>4.4807440005E10</c:v>
+                  <c:v>2.035274846E9</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>4.7651422505E10</c:v>
+                  <c:v>2.388506096E9</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>5.0582905005E10</c:v>
+                  <c:v>2.769987346E9</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>5.3601887505E10</c:v>
+                  <c:v>3.179718596E9</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>5.6708370005E10</c:v>
+                  <c:v>3.617699846E9</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>5.9902352505E10</c:v>
+                  <c:v>4.083931096E9</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>6.3183835005E10</c:v>
+                  <c:v>4.578412346E9</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>6.6552817505E10</c:v>
+                  <c:v>5.101143596E9</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>7.0009300005E10</c:v>
+                  <c:v>5.652124846E9</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>7.3553282505E10</c:v>
+                  <c:v>6.231356096E9</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>7.7184765005E10</c:v>
+                  <c:v>6.838837346E9</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>8.0903747505E10</c:v>
+                  <c:v>7.474568596E9</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>8.4710230005E10</c:v>
+                  <c:v>8.138549846E9</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>8.8604212505E10</c:v>
+                  <c:v>8.830781096E9</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>9.2585695005E10</c:v>
+                  <c:v>9.551262346E9</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>9.6654677505E10</c:v>
+                  <c:v>1.0299993596E10</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>1.00811160005E11</c:v>
+                  <c:v>1.1076974846E10</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>1.05055142505E11</c:v>
+                  <c:v>1.1882206096E10</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>1.09386625005E11</c:v>
+                  <c:v>1.2715687346E10</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1363,11 +1386,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2143997288"/>
-        <c:axId val="-2143994312"/>
+        <c:axId val="-2137226376"/>
+        <c:axId val="-2137223288"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2143997288"/>
+        <c:axId val="-2137226376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1377,7 +1400,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2143994312"/>
+        <c:crossAx val="-2137223288"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1385,7 +1408,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2143994312"/>
+        <c:axId val="-2137223288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1396,7 +1419,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2143997288"/>
+        <c:crossAx val="-2137226376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1555,97 +1578,97 @@
             <c:numRef>
               <c:f>'Configuración 3'!$B$12:$AE$12</c:f>
               <c:numCache>
-                <c:formatCode>#,##0.00;\-#,##0.00</c:formatCode>
+                <c:formatCode>#,##0;\-#,##0</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>2.27859800001E11</c:v>
+                  <c:v>2.3583429E7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.97611200001E11</c:v>
+                  <c:v>9.4166929E7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.76662600001E11</c:v>
+                  <c:v>2.11750429E8</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.65014000001E11</c:v>
+                  <c:v>3.76333929E8</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.62665400001E11</c:v>
+                  <c:v>5.87917429E8</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6.69616800001E11</c:v>
+                  <c:v>8.46500929E8</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7.85868200001E11</c:v>
+                  <c:v>1.152084429E9</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9.11419600001E11</c:v>
+                  <c:v>1.504667929E9</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.046271000001E12</c:v>
+                  <c:v>1.904251429E9</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.190422400001E12</c:v>
+                  <c:v>2.350834929E9</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.343873800001E12</c:v>
+                  <c:v>2.844418429E9</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.506625200001E12</c:v>
+                  <c:v>3.385001929E9</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.678676600001E12</c:v>
+                  <c:v>3.972585429E9</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.860028000001E12</c:v>
+                  <c:v>4.607168929E9</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2.050679400001E12</c:v>
+                  <c:v>5.288752429E9</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2.250630800001E12</c:v>
+                  <c:v>6.017335929E9</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2.459882200001E12</c:v>
+                  <c:v>6.792919429E9</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2.678433600001E12</c:v>
+                  <c:v>7.615502929E9</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2.906285000001E12</c:v>
+                  <c:v>8.485086429E9</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>3.143436400001E12</c:v>
+                  <c:v>9.401669929E9</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>3.389887800001E12</c:v>
+                  <c:v>1.0365253429E10</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>3.645639200001E12</c:v>
+                  <c:v>1.1375836929E10</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>3.910690600001E12</c:v>
+                  <c:v>1.2433420429E10</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>4.185042000001E12</c:v>
+                  <c:v>1.3538003929E10</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>4.468693400001E12</c:v>
+                  <c:v>1.4689587429E10</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>4.761644800001E12</c:v>
+                  <c:v>1.5888170929E10</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>5.063896200001E12</c:v>
+                  <c:v>1.7133754429E10</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>5.375447600001E12</c:v>
+                  <c:v>1.8426337929E10</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>5.696299000001E12</c:v>
+                  <c:v>1.9765921429E10</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>6.026450400001E12</c:v>
+                  <c:v>2.1152504929E10</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1772,94 +1795,94 @@
                 <c:formatCode>#,##0;\-#,##0</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>1.71514560001E11</c:v>
+                  <c:v>1.4231096E7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.24016640001E11</c:v>
+                  <c:v>5.6712346E7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.83518720001E11</c:v>
+                  <c:v>1.27443596E8</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.50020800001E11</c:v>
+                  <c:v>2.26424846E8</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.23522880001E11</c:v>
+                  <c:v>3.53656096E8</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.04024960001E11</c:v>
+                  <c:v>5.09137346E8</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5.91527040001E11</c:v>
+                  <c:v>6.92868596E8</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6.86029120001E11</c:v>
+                  <c:v>9.04849846E8</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>7.87531200001E11</c:v>
+                  <c:v>1.145081096E9</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>8.96033280001E11</c:v>
+                  <c:v>1.413562346E9</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.011535360001E12</c:v>
+                  <c:v>1.710293596E9</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.134037440001E12</c:v>
+                  <c:v>2.035274846E9</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.263539520001E12</c:v>
+                  <c:v>2.388506096E9</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.400041600001E12</c:v>
+                  <c:v>2.769987346E9</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.543543680001E12</c:v>
+                  <c:v>3.179718596E9</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1.694045760001E12</c:v>
+                  <c:v>3.617699846E9</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1.851547840001E12</c:v>
+                  <c:v>4.083931096E9</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2.016049920001E12</c:v>
+                  <c:v>4.578412346E9</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2.187552000001E12</c:v>
+                  <c:v>5.101143596E9</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2.366054080001E12</c:v>
+                  <c:v>5.652124846E9</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2.551556160001E12</c:v>
+                  <c:v>6.231356096E9</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2.744058240001E12</c:v>
+                  <c:v>6.838837346E9</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2.943560320001E12</c:v>
+                  <c:v>7.474568596E9</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>3.150062400001E12</c:v>
+                  <c:v>8.138549846E9</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>3.363564480001E12</c:v>
+                  <c:v>8.830781096E9</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>3.584066560001E12</c:v>
+                  <c:v>9.551262346E9</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>3.811568640001E12</c:v>
+                  <c:v>1.0299993596E10</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>4.046070720001E12</c:v>
+                  <c:v>1.1076974846E10</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>4.287572800001E12</c:v>
+                  <c:v>1.1882206096E10</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>4.536074880001E12</c:v>
+                  <c:v>1.2715687346E10</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1876,11 +1899,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2143917240"/>
-        <c:axId val="-2143914264"/>
+        <c:axId val="-2137144936"/>
+        <c:axId val="-2137141880"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2143917240"/>
+        <c:axId val="-2137144936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1890,7 +1913,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2143914264"/>
+        <c:crossAx val="-2137141880"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1898,18 +1921,18 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2143914264"/>
+        <c:axId val="-2137141880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
-        <c:numFmt formatCode="#,##0.00;\-#,##0.00" sourceLinked="1"/>
+        <c:numFmt formatCode="#,##0;\-#,##0" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2143917240"/>
+        <c:crossAx val="-2137144936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2071,94 +2094,94 @@
                 <c:formatCode>#,##0;\-#,##0</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>3.37610960008E11</c:v>
+                  <c:v>2.3583429E7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.27287330008E11</c:v>
+                  <c:v>9.4166929E7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.27513700008E11</c:v>
+                  <c:v>2.11750429E8</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.38290070008E11</c:v>
+                  <c:v>3.76333929E8</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.59616440008E11</c:v>
+                  <c:v>5.87917429E8</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8.91492810008E11</c:v>
+                  <c:v>8.46500929E8</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.033919180008E12</c:v>
+                  <c:v>1.152084429E9</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.186895550008E12</c:v>
+                  <c:v>1.504667929E9</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.350421920008E12</c:v>
+                  <c:v>1.904251429E9</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.524498290008E12</c:v>
+                  <c:v>2.350834929E9</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.709124660008E12</c:v>
+                  <c:v>2.844418429E9</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.904301030008E12</c:v>
+                  <c:v>3.385001929E9</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2.110027400008E12</c:v>
+                  <c:v>3.972585429E9</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2.326303770008E12</c:v>
+                  <c:v>4.607168929E9</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2.553130140008E12</c:v>
+                  <c:v>5.288752429E9</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2.790506510008E12</c:v>
+                  <c:v>6.017335929E9</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>3.038432880008E12</c:v>
+                  <c:v>6.792919429E9</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>3.296909250008E12</c:v>
+                  <c:v>7.615502929E9</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>3.565935620008E12</c:v>
+                  <c:v>8.485086429E9</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>3.845511990008E12</c:v>
+                  <c:v>9.401669929E9</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>4.135638360008E12</c:v>
+                  <c:v>1.0365253429E10</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>4.436314730008E12</c:v>
+                  <c:v>1.1375836929E10</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>4.747541100008E12</c:v>
+                  <c:v>1.2433420429E10</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>5.069317470008E12</c:v>
+                  <c:v>1.3538003929E10</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>5.401643840008E12</c:v>
+                  <c:v>1.4689587429E10</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>5.744520210008E12</c:v>
+                  <c:v>1.5888170929E10</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>6.097946580008E12</c:v>
+                  <c:v>1.7133754429E10</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>6.461922950008E12</c:v>
+                  <c:v>1.8426337929E10</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>6.836449320008E12</c:v>
+                  <c:v>1.9765921429E10</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>7.221525690008E12</c:v>
+                  <c:v>2.1152504929E10</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2285,94 +2308,94 @@
                 <c:formatCode>#,##0;\-#,##0</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>2.16012360008E11</c:v>
+                  <c:v>1.4231096E7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.73388905008E11</c:v>
+                  <c:v>5.6712346E7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.37515450008E11</c:v>
+                  <c:v>1.27443596E8</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.08391995008E11</c:v>
+                  <c:v>2.26424846E8</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.86018540008E11</c:v>
+                  <c:v>3.53656096E8</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.70395085008E11</c:v>
+                  <c:v>5.09137346E8</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6.61521630008E11</c:v>
+                  <c:v>6.92868596E8</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7.59398175008E11</c:v>
+                  <c:v>9.04849846E8</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8.64024720008E11</c:v>
+                  <c:v>1.145081096E9</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9.75401265008E11</c:v>
+                  <c:v>1.413562346E9</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.093527810008E12</c:v>
+                  <c:v>1.710293596E9</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.218404355008E12</c:v>
+                  <c:v>2.035274846E9</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.350030900008E12</c:v>
+                  <c:v>2.388506096E9</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.488407445008E12</c:v>
+                  <c:v>2.769987346E9</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.633533990008E12</c:v>
+                  <c:v>3.179718596E9</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1.785410535008E12</c:v>
+                  <c:v>3.617699846E9</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1.944037080008E12</c:v>
+                  <c:v>4.083931096E9</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2.109413625008E12</c:v>
+                  <c:v>4.578412346E9</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2.281540170008E12</c:v>
+                  <c:v>5.101143596E9</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2.460416715008E12</c:v>
+                  <c:v>5.652124846E9</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2.646043260008E12</c:v>
+                  <c:v>6.231356096E9</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2.838419805008E12</c:v>
+                  <c:v>6.838837346E9</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>3.037546350008E12</c:v>
+                  <c:v>7.474568596E9</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>3.243422895008E12</c:v>
+                  <c:v>8.138549846E9</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>3.456049440008E12</c:v>
+                  <c:v>8.830781096E9</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>3.675425985008E12</c:v>
+                  <c:v>9.551262346E9</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>3.901552530008E12</c:v>
+                  <c:v>1.0299993596E10</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>4.134429075008E12</c:v>
+                  <c:v>1.1076974846E10</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>4.374055620008E12</c:v>
+                  <c:v>1.1882206096E10</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>4.620432165008E12</c:v>
+                  <c:v>1.2715687346E10</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2389,11 +2412,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2144990488"/>
-        <c:axId val="-2144988168"/>
+        <c:axId val="-2137065288"/>
+        <c:axId val="-2137062216"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2144990488"/>
+        <c:axId val="-2137065288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2403,7 +2426,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2144988168"/>
+        <c:crossAx val="-2137062216"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2411,7 +2434,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2144988168"/>
+        <c:axId val="-2137062216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2422,7 +2445,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2144990488"/>
+        <c:crossAx val="-2137065288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2584,94 +2607,94 @@
                 <c:formatCode>#,##0;\-#,##0</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>7.74215330006E11</c:v>
+                  <c:v>2.3583429E7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8.88766425006E11</c:v>
+                  <c:v>9.4166929E7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.011217520006E12</c:v>
+                  <c:v>2.11750429E8</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.141568615006E12</c:v>
+                  <c:v>3.76333929E8</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.279819710006E12</c:v>
+                  <c:v>5.87917429E8</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.425970805006E12</c:v>
+                  <c:v>8.46500929E8</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.580021900006E12</c:v>
+                  <c:v>1.152084429E9</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.741972995006E12</c:v>
+                  <c:v>1.504667929E9</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.911824090006E12</c:v>
+                  <c:v>1.904251429E9</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.089575185006E12</c:v>
+                  <c:v>2.350834929E9</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.275226280006E12</c:v>
+                  <c:v>2.844418429E9</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2.468777375006E12</c:v>
+                  <c:v>3.385001929E9</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2.670228470006E12</c:v>
+                  <c:v>3.972585429E9</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2.879579565006E12</c:v>
+                  <c:v>4.607168929E9</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3.096830660006E12</c:v>
+                  <c:v>5.288752429E9</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>3.321981755006E12</c:v>
+                  <c:v>6.017335929E9</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>3.555032850006E12</c:v>
+                  <c:v>6.792919429E9</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>3.795983945006E12</c:v>
+                  <c:v>7.615502929E9</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>4.044835040006E12</c:v>
+                  <c:v>8.485086429E9</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>4.301586135006E12</c:v>
+                  <c:v>9.401669929E9</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>4.566237230006E12</c:v>
+                  <c:v>1.0365253429E10</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>4.838788325006E12</c:v>
+                  <c:v>1.1375836929E10</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>5.119239420006E12</c:v>
+                  <c:v>1.2433420429E10</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>5.407590515006E12</c:v>
+                  <c:v>1.3538003929E10</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>5.703841610006E12</c:v>
+                  <c:v>1.4689587429E10</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>6.007992705006E12</c:v>
+                  <c:v>1.5888170929E10</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>6.320043800006E12</c:v>
+                  <c:v>1.7133754429E10</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>6.639994895006E12</c:v>
+                  <c:v>1.8426337929E10</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>6.967845990006E12</c:v>
+                  <c:v>1.9765921429E10</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>7.303597085006E12</c:v>
+                  <c:v>2.1152504929E10</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2798,94 +2821,94 @@
                 <c:formatCode>#,##0;\-#,##0</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>5.04721210006E11</c:v>
+                  <c:v>1.4231096E7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.79397725006E11</c:v>
+                  <c:v>5.6712346E7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.59224240006E11</c:v>
+                  <c:v>1.27443596E8</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7.44200755006E11</c:v>
+                  <c:v>2.26424846E8</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8.34327270006E11</c:v>
+                  <c:v>3.53656096E8</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9.29603785006E11</c:v>
+                  <c:v>5.09137346E8</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.030030300006E12</c:v>
+                  <c:v>6.92868596E8</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.135606815006E12</c:v>
+                  <c:v>9.04849846E8</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.246333330006E12</c:v>
+                  <c:v>1.145081096E9</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.362209845006E12</c:v>
+                  <c:v>1.413562346E9</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.483236360006E12</c:v>
+                  <c:v>1.710293596E9</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.609412875006E12</c:v>
+                  <c:v>2.035274846E9</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.740739390006E12</c:v>
+                  <c:v>2.388506096E9</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.877215905006E12</c:v>
+                  <c:v>2.769987346E9</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2.018842420006E12</c:v>
+                  <c:v>3.179718596E9</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2.165618935006E12</c:v>
+                  <c:v>3.617699846E9</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2.317545450006E12</c:v>
+                  <c:v>4.083931096E9</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2.474621965006E12</c:v>
+                  <c:v>4.578412346E9</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2.636848480006E12</c:v>
+                  <c:v>5.101143596E9</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2.804224995006E12</c:v>
+                  <c:v>5.652124846E9</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2.976751510006E12</c:v>
+                  <c:v>6.231356096E9</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>3.154428025006E12</c:v>
+                  <c:v>6.838837346E9</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>3.337254540006E12</c:v>
+                  <c:v>7.474568596E9</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>3.525231055006E12</c:v>
+                  <c:v>8.138549846E9</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>3.718357570006E12</c:v>
+                  <c:v>8.830781096E9</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>3.916634085006E12</c:v>
+                  <c:v>9.551262346E9</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>4.120060600006E12</c:v>
+                  <c:v>1.0299993596E10</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>4.328637115006E12</c:v>
+                  <c:v>1.1076974846E10</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>4.542363630006E12</c:v>
+                  <c:v>1.1882206096E10</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>4.761240145006E12</c:v>
+                  <c:v>1.2715687346E10</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2902,11 +2925,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2144900392"/>
-        <c:axId val="-2144897416"/>
+        <c:axId val="-2137560328"/>
+        <c:axId val="-2137563400"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2144900392"/>
+        <c:axId val="-2137560328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2916,7 +2939,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2144897416"/>
+        <c:crossAx val="-2137563400"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2924,7 +2947,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2144897416"/>
+        <c:axId val="-2137563400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2935,7 +2958,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2144900392"/>
+        <c:crossAx val="-2137560328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2961,20 +2984,20 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>12700</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>863600</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
+      <xdr:rowOff>44450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>939800</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>139700</xdr:rowOff>
+      <xdr:colOff>901700</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="4" name="Chart 3"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -3456,21 +3479,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE16"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G14" sqref="G14"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
-    <col min="2" max="2" width="14.1640625" customWidth="1"/>
+    <col min="2" max="2" width="17" customWidth="1"/>
     <col min="3" max="3" width="13.5" style="20" customWidth="1"/>
     <col min="4" max="4" width="14.6640625" customWidth="1"/>
     <col min="5" max="5" width="12.6640625" customWidth="1"/>
     <col min="6" max="7" width="15.5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.83203125" style="20" bestFit="1" customWidth="1"/>
-    <col min="9" max="22" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="21" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="15.1640625" bestFit="1" customWidth="1"/>
     <col min="23" max="31" width="15.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3566,11 +3590,11 @@
         <v>7</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="20">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:31">
@@ -3580,99 +3604,105 @@
       <c r="C8" s="20">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:31" s="39" customFormat="1">
-      <c r="A10" s="38" t="s">
+      <c r="F8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H8" s="20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:31" s="36" customFormat="1">
+      <c r="A10" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="39">
+      <c r="B10" s="36">
         <v>500</v>
       </c>
-      <c r="C10" s="38">
+      <c r="C10" s="35">
         <v>1000</v>
       </c>
-      <c r="D10" s="39">
+      <c r="D10" s="36">
         <v>1500</v>
       </c>
-      <c r="E10" s="39">
+      <c r="E10" s="36">
         <v>2000</v>
       </c>
-      <c r="F10" s="39">
+      <c r="F10" s="36">
         <v>2500</v>
       </c>
-      <c r="G10" s="39">
+      <c r="G10" s="36">
         <v>3000</v>
       </c>
-      <c r="H10" s="38">
+      <c r="H10" s="35">
         <v>3500</v>
       </c>
-      <c r="I10" s="39">
+      <c r="I10" s="36">
         <v>4000</v>
       </c>
-      <c r="J10" s="39">
+      <c r="J10" s="36">
         <v>4500</v>
       </c>
-      <c r="K10" s="39">
+      <c r="K10" s="36">
         <v>5000</v>
       </c>
-      <c r="L10" s="39">
+      <c r="L10" s="36">
         <v>5500</v>
       </c>
-      <c r="M10" s="39">
+      <c r="M10" s="36">
         <v>6000</v>
       </c>
-      <c r="N10" s="39">
+      <c r="N10" s="36">
         <v>6500</v>
       </c>
-      <c r="O10" s="39">
+      <c r="O10" s="36">
         <v>7000</v>
       </c>
-      <c r="P10" s="39">
+      <c r="P10" s="36">
         <v>7500</v>
       </c>
-      <c r="Q10" s="39">
+      <c r="Q10" s="36">
         <v>8000</v>
       </c>
-      <c r="R10" s="39">
+      <c r="R10" s="36">
         <v>8500</v>
       </c>
-      <c r="S10" s="39">
+      <c r="S10" s="36">
         <v>9000</v>
       </c>
-      <c r="T10" s="39">
+      <c r="T10" s="36">
         <v>9500</v>
       </c>
-      <c r="U10" s="39">
+      <c r="U10" s="36">
         <v>10000</v>
       </c>
-      <c r="V10" s="39">
+      <c r="V10" s="36">
         <v>10500</v>
       </c>
-      <c r="W10" s="39">
+      <c r="W10" s="36">
         <v>11000</v>
       </c>
-      <c r="X10" s="39">
+      <c r="X10" s="36">
         <v>11500</v>
       </c>
-      <c r="Y10" s="39">
+      <c r="Y10" s="36">
         <v>12000</v>
       </c>
-      <c r="Z10" s="39">
+      <c r="Z10" s="36">
         <v>12500</v>
       </c>
-      <c r="AA10" s="39">
+      <c r="AA10" s="36">
         <v>13000</v>
       </c>
-      <c r="AB10" s="39">
+      <c r="AB10" s="36">
         <v>13500</v>
       </c>
-      <c r="AC10" s="39">
+      <c r="AC10" s="36">
         <v>14000</v>
       </c>
-      <c r="AD10" s="39">
+      <c r="AD10" s="36">
         <v>14500</v>
       </c>
-      <c r="AE10" s="39">
+      <c r="AE10" s="36">
         <v>15000</v>
       </c>
     </row>
@@ -3680,257 +3710,257 @@
       <c r="A11" s="10"/>
     </row>
     <row r="12" spans="1:31" s="29" customFormat="1" ht="15">
-      <c r="A12" s="32" t="s">
+      <c r="A12" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="29">
-        <f>(B10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*B10+C8</f>
-        <v>22306002</v>
+      <c r="B12" s="41">
+        <f>(B10-1)*(3*C3+C5+C6)+((B10*(B10+1)/2)*(4*C3+6*C4+2*C5+4*C7))+C8</f>
+        <v>23583429</v>
       </c>
       <c r="C12" s="29">
-        <f>(C10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*C10+C8</f>
-        <v>89112002</v>
+        <f>(C10-1)*(3*C3+C5+C6)+((C10*(C10+1)/2)*(4*C3+6*C4+2*C5+4*C7))+C8</f>
+        <v>94166929</v>
       </c>
       <c r="D12" s="29">
-        <f>(D10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*D10+C8</f>
-        <v>200418002</v>
+        <f>(D10-1)*(3*C3+C5+C6)+((D10*(D10+1)/2)*(4*C3+6*C4+2*C5+4*C7))+C8</f>
+        <v>211750429</v>
       </c>
       <c r="E12" s="29">
-        <f>(E10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*E10+C8</f>
-        <v>356224002</v>
+        <f>(E10-1)*(3*C3+C5+C6)+((E10*(E10+1)/2)*(4*C3+6*C4+2*C5+4*C7))+C8</f>
+        <v>376333929</v>
       </c>
       <c r="F12" s="29">
-        <f>(F10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*F10+C8</f>
-        <v>556530002</v>
+        <f>(F10-1)*(3*C3+C5+C6)+((F10*(F10+1)/2)*(4*C3+6*C4+2*C5+4*C7))+C8</f>
+        <v>587917429</v>
       </c>
       <c r="G12" s="29">
-        <f>(G10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*G10+C8</f>
-        <v>801336002</v>
+        <f>(G10-1)*(3*C3+C5+C6)+((G10*(G10+1)/2)*(4*C3+6*C4+2*C5+4*C7))+C8</f>
+        <v>846500929</v>
       </c>
       <c r="H12" s="29">
-        <f>(H10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*H10+C8</f>
-        <v>1090642002</v>
+        <f>(H10-1)*(3*C3+C5+C6)+((H10*(H10+1)/2)*(4*C3+6*C4+2*C5+4*C7))+C8</f>
+        <v>1152084429</v>
       </c>
       <c r="I12" s="29">
-        <f>(I10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*I10+C8</f>
-        <v>1424448002</v>
+        <f>(I10-1)*(3*C3+C5+C6)+((I10*(I10+1)/2)*(4*C3+6*C4+2*C5+4*C7))+C8</f>
+        <v>1504667929</v>
       </c>
       <c r="J12" s="29">
-        <f>(J10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*J10+C8</f>
-        <v>1802754002</v>
+        <f>(J10-1)*(3*C3+C5+C6)+((J10*(J10+1)/2)*(4*C3+6*C4+2*C5+4*C7))+C8</f>
+        <v>1904251429</v>
       </c>
       <c r="K12" s="29">
-        <f>(K10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*K10+C8</f>
-        <v>2225560002</v>
+        <f>(K10-1)*(3*C3+C5+C6)+((K10*(K10+1)/2)*(4*C3+6*C4+2*C5+4*C7))+C8</f>
+        <v>2350834929</v>
       </c>
       <c r="L12" s="29">
-        <f>(L10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*L10+C8</f>
-        <v>2692866002</v>
+        <f>(L10-1)*(3*C3+C5+C6)+((L10*(L10+1)/2)*(4*C3+6*C4+2*C5+4*C7))+C8</f>
+        <v>2844418429</v>
       </c>
       <c r="M12" s="29">
-        <f>(M10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*M10+C8</f>
-        <v>3204672002</v>
+        <f>(M10-1)*(3*C3+C5+C6)+((M10*(M10+1)/2)*(4*C3+6*C4+2*C5+4*C7))+C8</f>
+        <v>3385001929</v>
       </c>
       <c r="N12" s="29">
-        <f>(N10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*N10+C8</f>
-        <v>3760978002</v>
+        <f>(N10-1)*(3*C3+C5+C6)+((N10*(N10+1)/2)*(4*C3+6*C4+2*C5+4*C7))+C8</f>
+        <v>3972585429</v>
       </c>
       <c r="O12" s="29">
-        <f>(O10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*O10+C8</f>
-        <v>4361784002</v>
+        <f>(O10-1)*(3*C3+C5+C6)+((O10*(O10+1)/2)*(4*C3+6*C4+2*C5+4*C7))+C8</f>
+        <v>4607168929</v>
       </c>
       <c r="P12" s="29">
-        <f>(P10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*P10+C8</f>
-        <v>5007090002</v>
+        <f>(P10-1)*(3*C3+C5+C6)+((P10*(P10+1)/2)*(4*C3+6*C4+2*C5+4*C7))+C8</f>
+        <v>5288752429</v>
       </c>
       <c r="Q12" s="29">
-        <f>(Q10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*Q10+C8</f>
-        <v>5696896002</v>
+        <f>(Q10-1)*(3*C3+C5+C6)+((Q10*(Q10+1)/2)*(4*C3+6*C4+2*C5+4*C7))+C8</f>
+        <v>6017335929</v>
       </c>
       <c r="R12" s="29">
-        <f>(R10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*R10+C8</f>
-        <v>6431202002</v>
+        <f>(R10-1)*(3*C3+C5+C6)+((R10*(R10+1)/2)*(4*C3+6*C4+2*C5+4*C7))+C8</f>
+        <v>6792919429</v>
       </c>
       <c r="S12" s="29">
-        <f>(S10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*S10+C8</f>
-        <v>7210008002</v>
+        <f>(S10-1)*(3*C3+C5+C6)+((S10*(S10+1)/2)*(4*C3+6*C4+2*C5+4*C7))+C8</f>
+        <v>7615502929</v>
       </c>
       <c r="T12" s="29">
-        <f>(T10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*T10+C8</f>
-        <v>8033314002</v>
+        <f>(T10-1)*(3*C3+C5+C6)+((T10*(T10+1)/2)*(4*C3+6*C4+2*C5+4*C7))+C8</f>
+        <v>8485086429</v>
       </c>
       <c r="U12" s="29">
-        <f>(U10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*U10+C8</f>
-        <v>8901120002</v>
+        <f>(U10-1)*(3*C3+C5+C6)+((U10*(U10+1)/2)*(4*C3+6*C4+2*C5+4*C7))+C8</f>
+        <v>9401669929</v>
       </c>
       <c r="V12" s="29">
-        <f>(V10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*V10+C8</f>
-        <v>9813426002</v>
+        <f>(V10-1)*(3*C3+C5+C6)+((V10*(V10+1)/2)*(4*C3+6*C4+2*C5+4*C7))+C8</f>
+        <v>10365253429</v>
       </c>
       <c r="W12" s="29">
-        <f>(W10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*W10+C8</f>
-        <v>10770232002</v>
+        <f>(W10-1)*(3*C3+C5+C6)+((W10*(W10+1)/2)*(4*C3+6*C4+2*C5+4*C7))+C8</f>
+        <v>11375836929</v>
       </c>
       <c r="X12" s="29">
-        <f>(X10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*X10+C8</f>
-        <v>11771538002</v>
+        <f>(X10-1)*(3*C3+C5+C6)+((X10*(X10+1)/2)*(4*C3+6*C4+2*C5+4*C7))+C8</f>
+        <v>12433420429</v>
       </c>
       <c r="Y12" s="29">
-        <f>(Y10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*Y10+C8</f>
-        <v>12817344002</v>
+        <f>(Y10-1)*(3*C3+C5+C6)+((Y10*(Y10+1)/2)*(4*C3+6*C4+2*C5+4*C7))+C8</f>
+        <v>13538003929</v>
       </c>
       <c r="Z12" s="29">
-        <f>(Z10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*Z10+C8</f>
-        <v>13907650002</v>
+        <f>(Z10-1)*(3*C3+C5+C6)+((Z10*(Z10+1)/2)*(4*C3+6*C4+2*C5+4*C7))+C8</f>
+        <v>14689587429</v>
       </c>
       <c r="AA12" s="29">
-        <f>(AA10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*AA10+C8</f>
-        <v>15042456002</v>
+        <f>(AA10-1)*(3*C3+C5+C6)+((AA10*(AA10+1)/2)*(4*C3+6*C4+2*C5+4*C7))+C8</f>
+        <v>15888170929</v>
       </c>
       <c r="AB12" s="29">
-        <f>(AB10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*AB10+C8</f>
-        <v>16221762002</v>
+        <f>(AB10-1)*(3*C3+C5+C6)+((AB10*(AB10+1)/2)*(4*C3+6*C4+2*C5+4*C7))+C8</f>
+        <v>17133754429</v>
       </c>
       <c r="AC12" s="29">
-        <f>(AC10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*AC10+C8</f>
-        <v>17445568002</v>
+        <f>(AC10-1)*(3*C3+C5+C6)+((AC10*(AC10+1)/2)*(4*C3+6*C4+2*C5+4*C7))+C8</f>
+        <v>18426337929</v>
       </c>
       <c r="AD12" s="29">
-        <f>(AD10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*AD10+C8</f>
-        <v>18713874002</v>
+        <f>(AD10-1)*(3*C3+C5+C6)+((AD10*(AD10+1)/2)*(4*C3+6*C4+2*C5+4*C7))+C8</f>
+        <v>19765921429</v>
       </c>
       <c r="AE12" s="29">
-        <f>(AE10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*AE10+C8</f>
-        <v>20026680002</v>
+        <f>(AE10-1)*(3*C3+C5+C6)+((AE10*(AE10+1)/2)*(4*C3+6*C4+2*C5+4*C7))+C8</f>
+        <v>21152504929</v>
       </c>
     </row>
     <row r="14" spans="1:31" s="29" customFormat="1" ht="15">
-      <c r="A14" s="32" t="s">
+      <c r="A14" s="30" t="s">
         <v>2</v>
       </c>
       <c r="B14" s="29">
-        <f>(B10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*B10+H7</f>
-        <v>13817502</v>
+        <f>(B10-1)*(5*H3+4*H4+H5+3*H7)+(B10*(B10+1)/2)*(3*H3+2*H4+2*H5+H6)+H8</f>
+        <v>14231096</v>
       </c>
       <c r="C14" s="29">
-        <f>(C10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*C10+H7</f>
-        <v>55135002</v>
+        <f>(C10-1)*(5*H3+4*H4+H5+3*H7)+(C10*(C10+1)/2)*(3*H3+2*H4+2*H5+H6)+H8</f>
+        <v>56712346</v>
       </c>
       <c r="D14" s="29">
-        <f>(D10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*D10+H7</f>
-        <v>123952502</v>
+        <f>(D10-1)*(5*H3+4*H4+H5+3*H7)+(D10*(D10+1)/2)*(3*H3+2*H4+2*H5+H6)+H8</f>
+        <v>127443596</v>
       </c>
       <c r="E14" s="29">
-        <f>(E10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*E10+H7</f>
-        <v>220270002</v>
+        <f>(E10-1)*(5*H3+4*H4+H5+3*H7)+(E10*(E10+1)/2)*(3*H3+2*H4+2*H5+H6)+H8</f>
+        <v>226424846</v>
       </c>
       <c r="F14" s="29">
-        <f>(F10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*F10+H7</f>
-        <v>344087502</v>
+        <f>(F10-1)*(5*H3+4*H4+H5+3*H7)+(F10*(F10+1)/2)*(3*H3+2*H4+2*H5+H6)+H8</f>
+        <v>353656096</v>
       </c>
       <c r="G14" s="29">
-        <f>(G10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*G10+H7</f>
-        <v>495405002</v>
+        <f>(G10-1)*(5*H3+4*H4+H5+3*H7)+(G10*(G10+1)/2)*(3*H3+2*H4+2*H5+H6)+H8</f>
+        <v>509137346</v>
       </c>
       <c r="H14" s="29">
-        <f>(H10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*H10+H7</f>
-        <v>674222502</v>
+        <f>(H10-1)*(5*H3+4*H4+H5+3*H7)+(H10*(H10+1)/2)*(3*H3+2*H4+2*H5+H6)+H8</f>
+        <v>692868596</v>
       </c>
       <c r="I14" s="29">
-        <f>(I10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*I10+H7</f>
-        <v>880540002</v>
+        <f>(I10-1)*(5*H3+4*H4+H5+3*H7)+(I10*(I10+1)/2)*(3*H3+2*H4+2*H5+H6)+H8</f>
+        <v>904849846</v>
       </c>
       <c r="J14" s="29">
-        <f>(J10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*J10+H7</f>
-        <v>1114357502</v>
+        <f>(J10-1)*(5*H3+4*H4+H5+3*H7)+(J10*(J10+1)/2)*(3*H3+2*H4+2*H5+H6)+H8</f>
+        <v>1145081096</v>
       </c>
       <c r="K14" s="29">
-        <f>(K10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*K10+H7</f>
-        <v>1375675002</v>
+        <f>(K10-1)*(5*H3+4*H4+H5+3*H7)+(K10*(K10+1)/2)*(3*H3+2*H4+2*H5+H6)+H8</f>
+        <v>1413562346</v>
       </c>
       <c r="L14" s="29">
-        <f>(L10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*L10+H7</f>
-        <v>1664492502</v>
+        <f>(L10-1)*(5*H3+4*H4+H5+3*H7)+(L10*(L10+1)/2)*(3*H3+2*H4+2*H5+H6)+H8</f>
+        <v>1710293596</v>
       </c>
       <c r="M14" s="29">
-        <f>(M10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*M10+H7</f>
-        <v>1980810002</v>
+        <f>(M10-1)*(5*H3+4*H4+H5+3*H7)+(M10*(M10+1)/2)*(3*H3+2*H4+2*H5+H6)+H8</f>
+        <v>2035274846</v>
       </c>
       <c r="N14" s="29">
-        <f>(N10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*N10+H7</f>
-        <v>2324627502</v>
+        <f>(N10-1)*(5*H3+4*H4+H5+3*H7)+(N10*(N10+1)/2)*(3*H3+2*H4+2*H5+H6)+H8</f>
+        <v>2388506096</v>
       </c>
       <c r="O14" s="29">
-        <f>(O10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*O10+H7</f>
-        <v>2695945002</v>
+        <f>(O10-1)*(5*H3+4*H4+H5+3*H7)+(O10*(O10+1)/2)*(3*H3+2*H4+2*H5+H6)+H8</f>
+        <v>2769987346</v>
       </c>
       <c r="P14" s="29">
-        <f>(P10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*P10+H7</f>
-        <v>3094762502</v>
+        <f>(P10-1)*(5*H3+4*H4+H5+3*H7)+(P10*(P10+1)/2)*(3*H3+2*H4+2*H5+H6)+H8</f>
+        <v>3179718596</v>
       </c>
       <c r="Q14" s="29">
-        <f>(Q10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*Q10+H7</f>
-        <v>3521080002</v>
+        <f>(Q10-1)*(5*H3+4*H4+H5+3*H7)+(Q10*(Q10+1)/2)*(3*H3+2*H4+2*H5+H6)+H8</f>
+        <v>3617699846</v>
       </c>
       <c r="R14" s="29">
-        <f>(R10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*R10+H7</f>
-        <v>3974897502</v>
+        <f>(R10-1)*(5*H3+4*H4+H5+3*H7)+(R10*(R10+1)/2)*(3*H3+2*H4+2*H5+H6)+H8</f>
+        <v>4083931096</v>
       </c>
       <c r="S14" s="29">
-        <f>(S10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*S10+H7</f>
-        <v>4456215002</v>
+        <f>(S10-1)*(5*H3+4*H4+H5+3*H7)+(S10*(S10+1)/2)*(3*H3+2*H4+2*H5+H6)+H8</f>
+        <v>4578412346</v>
       </c>
       <c r="T14" s="29">
-        <f>(T10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*T10+H7</f>
-        <v>4965032502</v>
+        <f>(T10-1)*(5*H3+4*H4+H5+3*H7)+(T10*(T10+1)/2)*(3*H3+2*H4+2*H5+H6)+H8</f>
+        <v>5101143596</v>
       </c>
       <c r="U14" s="29">
-        <f>(U10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*U10+H7</f>
-        <v>5501350002</v>
+        <f>(U10-1)*(5*H3+4*H4+H5+3*H7)+(U10*(U10+1)/2)*(3*H3+2*H4+2*H5+H6)+H8</f>
+        <v>5652124846</v>
       </c>
       <c r="V14" s="29">
-        <f>(V10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*V10+H7</f>
-        <v>6065167502</v>
+        <f>(V10-1)*(5*H3+4*H4+H5+3*H7)+(V10*(V10+1)/2)*(3*H3+2*H4+2*H5+H6)+H8</f>
+        <v>6231356096</v>
       </c>
       <c r="W14" s="29">
-        <f>(W10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*W10+H7</f>
-        <v>6656485002</v>
+        <f>(W10-1)*(5*H3+4*H4+H5+3*H7)+(W10*(W10+1)/2)*(3*H3+2*H4+2*H5+H6)+H8</f>
+        <v>6838837346</v>
       </c>
       <c r="X14" s="29">
-        <f>(X10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*X10+H7</f>
-        <v>7275302502</v>
+        <f>(X10-1)*(5*H3+4*H4+H5+3*H7)+(X10*(X10+1)/2)*(3*H3+2*H4+2*H5+H6)+H8</f>
+        <v>7474568596</v>
       </c>
       <c r="Y14" s="29">
-        <f>(Y10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*Y10+H7</f>
-        <v>7921620002</v>
+        <f>(Y10-1)*(5*H3+4*H4+H5+3*H7)+(Y10*(Y10+1)/2)*(3*H3+2*H4+2*H5+H6)+H8</f>
+        <v>8138549846</v>
       </c>
       <c r="Z14" s="29">
-        <f>(Z10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*Z10+H7</f>
-        <v>8595437502</v>
+        <f>(Z10-1)*(5*H3+4*H4+H5+3*H7)+(Z10*(Z10+1)/2)*(3*H3+2*H4+2*H5+H6)+H8</f>
+        <v>8830781096</v>
       </c>
       <c r="AA14" s="29">
-        <f>(AA10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*AA10+H7</f>
-        <v>9296755002</v>
+        <f>(AA10-1)*(5*H3+4*H4+H5+3*H7)+(AA10*(AA10+1)/2)*(3*H3+2*H4+2*H5+H6)+H8</f>
+        <v>9551262346</v>
       </c>
       <c r="AB14" s="29">
-        <f>(AB10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*AB10+H7</f>
-        <v>10025572502</v>
+        <f>(AB10-1)*(5*H3+4*H4+H5+3*H7)+(AB10*(AB10+1)/2)*(3*H3+2*H4+2*H5+H6)+H8</f>
+        <v>10299993596</v>
       </c>
       <c r="AC14" s="29">
-        <f>(AC10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*AC10+H7</f>
-        <v>10781890002</v>
+        <f>(AC10-1)*(5*H3+4*H4+H5+3*H7)+(AC10*(AC10+1)/2)*(3*H3+2*H4+2*H5+H6)+H8</f>
+        <v>11076974846</v>
       </c>
       <c r="AD14" s="29">
-        <f>(AD10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*AD10+H7</f>
-        <v>11565707502</v>
+        <f>(AD10-1)*(5*H3+4*H4+H5+3*H7)+(AD10*(AD10+1)/2)*(3*H3+2*H4+2*H5+H6)+H8</f>
+        <v>11882206096</v>
       </c>
       <c r="AE14" s="29">
-        <f>(AE10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*AE10+H7</f>
-        <v>12377025002</v>
+        <f>(AE10-1)*(5*H3+4*H4+H5+3*H7)+(AE10*(AE10+1)/2)*(3*H3+2*H4+2*H5+H6)+H8</f>
+        <v>12715687346</v>
       </c>
     </row>
     <row r="16" spans="1:31" ht="20">
-      <c r="D16" s="37" t="s">
+      <c r="D16" s="34" t="s">
         <v>13</v>
       </c>
     </row>
@@ -3950,9 +3980,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE17"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0"/>
@@ -4075,7 +4105,7 @@
         <v>5</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="20">
@@ -4089,104 +4119,109 @@
       <c r="C8" s="20">
         <v>5</v>
       </c>
-      <c r="H8" s="20"/>
+      <c r="F8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H8" s="20">
+        <v>5</v>
+      </c>
     </row>
     <row r="9" spans="1:31">
       <c r="C9" s="20"/>
       <c r="H9" s="20"/>
     </row>
-    <row r="10" spans="1:31" s="43" customFormat="1">
-      <c r="A10" s="42" t="s">
+    <row r="10" spans="1:31" s="38" customFormat="1">
+      <c r="A10" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="43">
+      <c r="B10" s="38">
         <v>10000</v>
       </c>
-      <c r="C10" s="42">
+      <c r="C10" s="37">
         <v>10500</v>
       </c>
-      <c r="D10" s="43">
+      <c r="D10" s="38">
         <v>11000</v>
       </c>
-      <c r="E10" s="43">
+      <c r="E10" s="38">
         <v>11500</v>
       </c>
-      <c r="F10" s="43">
+      <c r="F10" s="38">
         <v>12500</v>
       </c>
-      <c r="G10" s="43">
+      <c r="G10" s="38">
         <v>13000</v>
       </c>
-      <c r="H10" s="42">
+      <c r="H10" s="37">
         <v>13500</v>
       </c>
-      <c r="I10" s="43">
+      <c r="I10" s="38">
         <v>14000</v>
       </c>
-      <c r="J10" s="43">
+      <c r="J10" s="38">
         <v>14500</v>
       </c>
-      <c r="K10" s="43">
+      <c r="K10" s="38">
         <v>15000</v>
       </c>
-      <c r="L10" s="43">
+      <c r="L10" s="38">
         <v>15500</v>
       </c>
-      <c r="M10" s="43">
+      <c r="M10" s="38">
         <v>16000</v>
       </c>
-      <c r="N10" s="43">
+      <c r="N10" s="38">
         <v>16500</v>
       </c>
-      <c r="O10" s="43">
+      <c r="O10" s="38">
         <v>17000</v>
       </c>
-      <c r="P10" s="43">
+      <c r="P10" s="38">
         <v>17500</v>
       </c>
-      <c r="Q10" s="43">
+      <c r="Q10" s="38">
         <v>18000</v>
       </c>
-      <c r="R10" s="43">
+      <c r="R10" s="38">
         <v>18500</v>
       </c>
-      <c r="S10" s="43">
+      <c r="S10" s="38">
         <v>19000</v>
       </c>
-      <c r="T10" s="43">
+      <c r="T10" s="38">
         <v>19500</v>
       </c>
-      <c r="U10" s="43">
+      <c r="U10" s="38">
         <v>20000</v>
       </c>
-      <c r="V10" s="43">
+      <c r="V10" s="38">
         <v>20500</v>
       </c>
-      <c r="W10" s="43">
+      <c r="W10" s="38">
         <v>21000</v>
       </c>
-      <c r="X10" s="43">
+      <c r="X10" s="38">
         <v>21500</v>
       </c>
-      <c r="Y10" s="43">
+      <c r="Y10" s="38">
         <v>22000</v>
       </c>
-      <c r="Z10" s="43">
+      <c r="Z10" s="38">
         <v>22500</v>
       </c>
-      <c r="AA10" s="43">
+      <c r="AA10" s="38">
         <v>23000</v>
       </c>
-      <c r="AB10" s="43">
+      <c r="AB10" s="38">
         <v>23500</v>
       </c>
-      <c r="AC10" s="43">
+      <c r="AC10" s="38">
         <v>24000</v>
       </c>
-      <c r="AD10" s="43">
+      <c r="AD10" s="38">
         <v>24500</v>
       </c>
-      <c r="AE10" s="43">
+      <c r="AE10" s="38">
         <v>25000</v>
       </c>
     </row>
@@ -4195,129 +4230,99 @@
       <c r="C11" s="20"/>
       <c r="H11" s="20"/>
     </row>
-    <row r="12" spans="1:31" s="30" customFormat="1" ht="15">
-      <c r="A12" s="31" t="s">
+    <row r="12" spans="1:31" s="29" customFormat="1" ht="15">
+      <c r="A12" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="30">
-        <f>(B10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*B10+C8</f>
-        <v>22003700005</v>
-      </c>
-      <c r="C12" s="30">
-        <f>(C10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*C10+C8</f>
-        <v>24258885005</v>
-      </c>
-      <c r="D12" s="30">
-        <f>(D10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*D10+C8</f>
-        <v>26624070005</v>
-      </c>
-      <c r="E12" s="30">
-        <f>(E10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*E10+C8</f>
-        <v>29099255005</v>
-      </c>
-      <c r="F12" s="30">
-        <f>(F10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*F10+C8</f>
-        <v>34379625005</v>
-      </c>
-      <c r="G12" s="30">
-        <f>(G10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*G10+C8</f>
-        <v>37184810005</v>
-      </c>
-      <c r="H12" s="30">
-        <f>(H10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*H10+C8</f>
-        <v>40099995005</v>
-      </c>
-      <c r="I12" s="30">
-        <f>(I10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*I10+C8</f>
-        <v>43125180005</v>
-      </c>
-      <c r="J12" s="30">
-        <f>(J10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*J10+C8</f>
-        <v>46260365005</v>
-      </c>
-      <c r="K12" s="30">
-        <f>(K10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*K10+C8</f>
-        <v>49505550005</v>
-      </c>
-      <c r="L12" s="30">
-        <f>(L10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*L10+C8</f>
-        <v>52860735005</v>
-      </c>
-      <c r="M12" s="30">
-        <f>(M10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*M10+C8</f>
-        <v>56325920005</v>
-      </c>
-      <c r="N12" s="30">
-        <f>(N10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*N10+C8</f>
-        <v>59901105005</v>
-      </c>
-      <c r="O12" s="30">
-        <f>(O10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*O10+C8</f>
-        <v>63586290005</v>
-      </c>
-      <c r="P12" s="30">
-        <f>(P10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*P10+C8</f>
-        <v>67381475005</v>
-      </c>
-      <c r="Q12" s="30">
-        <f>(Q10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*Q10+C8</f>
-        <v>71286660005</v>
-      </c>
-      <c r="R12" s="30">
-        <f>(R10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*R10+C8</f>
-        <v>75301845005</v>
-      </c>
-      <c r="S12" s="30">
-        <f>(S10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*S10+C8</f>
-        <v>79427030005</v>
-      </c>
-      <c r="T12" s="30">
-        <f>(T10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*T10+C8</f>
-        <v>83662215005</v>
-      </c>
-      <c r="U12" s="30">
-        <f>(U10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*U10+C8</f>
-        <v>88007400005</v>
-      </c>
-      <c r="V12" s="30">
-        <f>(V10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*V10+C8</f>
-        <v>92462585005</v>
-      </c>
-      <c r="W12" s="30">
-        <f>(W10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*W10+C8</f>
-        <v>97027770005</v>
-      </c>
-      <c r="X12" s="30">
-        <f>(X10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*X10+C8</f>
-        <v>101702955005</v>
-      </c>
-      <c r="Y12" s="30">
-        <f>(Y10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*Y10+C8</f>
-        <v>106488140005</v>
-      </c>
-      <c r="Z12" s="30">
-        <f>(Z10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*Z10+C8</f>
-        <v>111383325005</v>
-      </c>
-      <c r="AA12" s="30">
-        <f>(AA10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*AA10+C8</f>
-        <v>116388510005</v>
-      </c>
-      <c r="AB12" s="30">
-        <f>(AB10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*AB10+C8</f>
-        <v>121503695005</v>
-      </c>
-      <c r="AC12" s="30">
-        <f>(AC10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*AC10+C8</f>
-        <v>126728880005</v>
-      </c>
-      <c r="AD12" s="30">
-        <f>(AD10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*AD10+C8</f>
-        <v>132064065005</v>
-      </c>
-      <c r="AE12" s="30">
-        <f>(AE10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*AE10+C8</f>
-        <v>137509250005</v>
+      <c r="B12" s="41">
+        <v>23583429</v>
+      </c>
+      <c r="C12" s="29">
+        <v>94166929</v>
+      </c>
+      <c r="D12" s="29">
+        <v>211750429</v>
+      </c>
+      <c r="E12" s="29">
+        <v>376333929</v>
+      </c>
+      <c r="F12" s="29">
+        <v>587917429</v>
+      </c>
+      <c r="G12" s="29">
+        <v>846500929</v>
+      </c>
+      <c r="H12" s="29">
+        <v>1152084429</v>
+      </c>
+      <c r="I12" s="29">
+        <v>1504667929</v>
+      </c>
+      <c r="J12" s="29">
+        <v>1904251429</v>
+      </c>
+      <c r="K12" s="29">
+        <v>2350834929</v>
+      </c>
+      <c r="L12" s="29">
+        <v>2844418429</v>
+      </c>
+      <c r="M12" s="29">
+        <v>3385001929</v>
+      </c>
+      <c r="N12" s="29">
+        <v>3972585429</v>
+      </c>
+      <c r="O12" s="29">
+        <v>4607168929</v>
+      </c>
+      <c r="P12" s="29">
+        <v>5288752429</v>
+      </c>
+      <c r="Q12" s="29">
+        <v>6017335929</v>
+      </c>
+      <c r="R12" s="29">
+        <v>6792919429</v>
+      </c>
+      <c r="S12" s="29">
+        <v>7615502929</v>
+      </c>
+      <c r="T12" s="29">
+        <v>8485086429</v>
+      </c>
+      <c r="U12" s="29">
+        <v>9401669929</v>
+      </c>
+      <c r="V12" s="29">
+        <v>10365253429</v>
+      </c>
+      <c r="W12" s="29">
+        <v>11375836929</v>
+      </c>
+      <c r="X12" s="29">
+        <v>12433420429</v>
+      </c>
+      <c r="Y12" s="29">
+        <v>13538003929</v>
+      </c>
+      <c r="Z12" s="29">
+        <v>14689587429</v>
+      </c>
+      <c r="AA12" s="29">
+        <v>15888170929</v>
+      </c>
+      <c r="AB12" s="29">
+        <v>17133754429</v>
+      </c>
+      <c r="AC12" s="29">
+        <v>18426337929</v>
+      </c>
+      <c r="AD12" s="29">
+        <v>19765921429</v>
+      </c>
+      <c r="AE12" s="29">
+        <v>21152504929</v>
       </c>
     </row>
     <row r="13" spans="1:31">
@@ -4325,128 +4330,98 @@
       <c r="H13" s="20"/>
     </row>
     <row r="14" spans="1:31" s="29" customFormat="1" ht="15">
-      <c r="A14" s="32" t="s">
+      <c r="A14" s="30" t="s">
         <v>2</v>
       </c>
       <c r="B14" s="29">
-        <f>(B10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*B10+H7</f>
-        <v>17504650005</v>
+        <v>14231096</v>
       </c>
       <c r="C14" s="29">
-        <f>(C10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*C10+H7</f>
-        <v>19298632505</v>
+        <v>56712346</v>
       </c>
       <c r="D14" s="29">
-        <f>(D10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*D10+H7</f>
-        <v>21180115005</v>
+        <v>127443596</v>
       </c>
       <c r="E14" s="29">
-        <f>(E10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*E10+H7</f>
-        <v>23149097505</v>
+        <v>226424846</v>
       </c>
       <c r="F14" s="29">
-        <f>(F10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*F10+H7</f>
-        <v>27349562505</v>
+        <v>353656096</v>
       </c>
       <c r="G14" s="29">
-        <f>(G10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*G10+H7</f>
-        <v>29581045005</v>
+        <v>509137346</v>
       </c>
       <c r="H14" s="29">
-        <f>(H10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*H10+H7</f>
-        <v>31900027505</v>
+        <v>692868596</v>
       </c>
       <c r="I14" s="29">
-        <f>(I10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*I10+H7</f>
-        <v>34306510005</v>
+        <v>904849846</v>
       </c>
       <c r="J14" s="29">
-        <f>(J10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*J10+H7</f>
-        <v>36800492505</v>
+        <v>1145081096</v>
       </c>
       <c r="K14" s="29">
-        <f>(K10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*K10+H7</f>
-        <v>39381975005</v>
+        <v>1413562346</v>
       </c>
       <c r="L14" s="29">
-        <f>(L10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*L10+H7</f>
-        <v>42050957505</v>
+        <v>1710293596</v>
       </c>
       <c r="M14" s="29">
-        <f>(M10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*M10+H7</f>
-        <v>44807440005</v>
+        <v>2035274846</v>
       </c>
       <c r="N14" s="29">
-        <f>(N10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*N10+H7</f>
-        <v>47651422505</v>
+        <v>2388506096</v>
       </c>
       <c r="O14" s="29">
-        <f>(O10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*O10+H7</f>
-        <v>50582905005</v>
+        <v>2769987346</v>
       </c>
       <c r="P14" s="29">
-        <f>(P10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*P10+H7</f>
-        <v>53601887505</v>
+        <v>3179718596</v>
       </c>
       <c r="Q14" s="29">
-        <f>(Q10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*Q10+H7</f>
-        <v>56708370005</v>
+        <v>3617699846</v>
       </c>
       <c r="R14" s="29">
-        <f>(R10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*R10+H7</f>
-        <v>59902352505</v>
+        <v>4083931096</v>
       </c>
       <c r="S14" s="29">
-        <f>(S10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*S10+H7</f>
-        <v>63183835005</v>
+        <v>4578412346</v>
       </c>
       <c r="T14" s="29">
-        <f>(T10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*T10+H7</f>
-        <v>66552817505</v>
+        <v>5101143596</v>
       </c>
       <c r="U14" s="29">
-        <f>(U10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*U10+H7</f>
-        <v>70009300005</v>
+        <v>5652124846</v>
       </c>
       <c r="V14" s="29">
-        <f>(V10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*V10+H7</f>
-        <v>73553282505</v>
+        <v>6231356096</v>
       </c>
       <c r="W14" s="29">
-        <f>(W10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*W10+H7</f>
-        <v>77184765005</v>
+        <v>6838837346</v>
       </c>
       <c r="X14" s="29">
-        <f>(X10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*X10+H7</f>
-        <v>80903747505</v>
+        <v>7474568596</v>
       </c>
       <c r="Y14" s="29">
-        <f>(Y10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*Y10+H7</f>
-        <v>84710230005</v>
+        <v>8138549846</v>
       </c>
       <c r="Z14" s="29">
-        <f>(Z10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*Z10+H7</f>
-        <v>88604212505</v>
+        <v>8830781096</v>
       </c>
       <c r="AA14" s="29">
-        <f>(AA10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*AA10+H7</f>
-        <v>92585695005</v>
+        <v>9551262346</v>
       </c>
       <c r="AB14" s="29">
-        <f>(AB10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*AB10+H7</f>
-        <v>96654677505</v>
+        <v>10299993596</v>
       </c>
       <c r="AC14" s="29">
-        <f>(AC10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*AC10+H7</f>
-        <v>100811160005</v>
+        <v>11076974846</v>
       </c>
       <c r="AD14" s="29">
-        <f>(AD10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*AD10+H7</f>
-        <v>105055142505</v>
+        <v>11882206096</v>
       </c>
       <c r="AE14" s="29">
-        <f>(AE10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*AE10+H7</f>
-        <v>109386625005</v>
+        <v>12715687346</v>
       </c>
     </row>
     <row r="15" spans="1:31">
@@ -4454,7 +4429,7 @@
       <c r="H15" s="20"/>
     </row>
     <row r="17" spans="4:4" ht="20">
-      <c r="D17" s="35" t="s">
+      <c r="D17" s="32" t="s">
         <v>13</v>
       </c>
     </row>
@@ -4475,8 +4450,8 @@
   <dimension ref="A1:AE16"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H26" sqref="H26"/>
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A12" sqref="A12:XFD14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4650,98 +4625,98 @@
       <c r="G9" s="12"/>
       <c r="H9" s="25"/>
     </row>
-    <row r="10" spans="1:31" s="39" customFormat="1" ht="17">
-      <c r="A10" s="38" t="s">
+    <row r="10" spans="1:31" s="36" customFormat="1" ht="17">
+      <c r="A10" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="39">
+      <c r="B10" s="36">
         <v>35000</v>
       </c>
-      <c r="C10" s="38">
+      <c r="C10" s="35">
         <v>40000</v>
       </c>
-      <c r="D10" s="39">
+      <c r="D10" s="36">
         <v>45000</v>
       </c>
-      <c r="E10" s="39">
+      <c r="E10" s="36">
         <v>50000</v>
       </c>
-      <c r="F10" s="39">
+      <c r="F10" s="36">
         <v>55000</v>
       </c>
-      <c r="G10" s="39">
+      <c r="G10" s="36">
         <v>60000</v>
       </c>
-      <c r="H10" s="38">
+      <c r="H10" s="35">
         <v>65000</v>
       </c>
-      <c r="I10" s="39">
+      <c r="I10" s="36">
         <v>70000</v>
       </c>
-      <c r="J10" s="39">
+      <c r="J10" s="36">
         <v>75000</v>
       </c>
-      <c r="K10" s="39">
+      <c r="K10" s="36">
         <v>80000</v>
       </c>
-      <c r="L10" s="39">
+      <c r="L10" s="36">
         <v>85000</v>
       </c>
-      <c r="M10" s="39">
+      <c r="M10" s="36">
         <v>90000</v>
       </c>
-      <c r="N10" s="39">
+      <c r="N10" s="36">
         <v>95000</v>
       </c>
-      <c r="O10" s="39">
+      <c r="O10" s="36">
         <v>100000</v>
       </c>
-      <c r="P10" s="39">
+      <c r="P10" s="36">
         <v>105000</v>
       </c>
-      <c r="Q10" s="39">
+      <c r="Q10" s="36">
         <v>110000</v>
       </c>
-      <c r="R10" s="39">
+      <c r="R10" s="36">
         <v>115000</v>
       </c>
-      <c r="S10" s="39">
+      <c r="S10" s="36">
         <v>120000</v>
       </c>
-      <c r="T10" s="39">
+      <c r="T10" s="36">
         <v>125000</v>
       </c>
-      <c r="U10" s="39">
+      <c r="U10" s="36">
         <v>130000</v>
       </c>
-      <c r="V10" s="39">
+      <c r="V10" s="36">
         <v>135000</v>
       </c>
-      <c r="W10" s="39">
+      <c r="W10" s="36">
         <v>140000</v>
       </c>
-      <c r="X10" s="39">
+      <c r="X10" s="36">
         <v>145000</v>
       </c>
-      <c r="Y10" s="39">
+      <c r="Y10" s="36">
         <v>150000</v>
       </c>
-      <c r="Z10" s="39">
+      <c r="Z10" s="36">
         <v>155000</v>
       </c>
-      <c r="AA10" s="39">
+      <c r="AA10" s="36">
         <v>160000</v>
       </c>
-      <c r="AB10" s="39">
+      <c r="AB10" s="36">
         <v>165000</v>
       </c>
-      <c r="AC10" s="39">
+      <c r="AC10" s="36">
         <v>170000</v>
       </c>
-      <c r="AD10" s="39">
+      <c r="AD10" s="36">
         <v>175000</v>
       </c>
-      <c r="AE10" s="39">
+      <c r="AE10" s="36">
         <v>180000</v>
       </c>
     </row>
@@ -4755,264 +4730,198 @@
       <c r="G11" s="12"/>
       <c r="H11" s="25"/>
     </row>
-    <row r="12" spans="1:31" s="41" customFormat="1">
-      <c r="A12" s="33" t="s">
+    <row r="12" spans="1:31" s="29" customFormat="1">
+      <c r="A12" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="40">
-        <f>(B10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*B10+C8</f>
-        <v>227859800001</v>
-      </c>
-      <c r="C12" s="40">
-        <f>(C10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*C10+C8</f>
-        <v>297611200001</v>
-      </c>
-      <c r="D12" s="40">
-        <f>(D10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*D10+C8</f>
-        <v>376662600001</v>
-      </c>
-      <c r="E12" s="40">
-        <f>(E10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*E10+C8</f>
-        <v>465014000001</v>
-      </c>
-      <c r="F12" s="40">
-        <f>(F10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*F10+C8</f>
-        <v>562665400001</v>
-      </c>
-      <c r="G12" s="40">
-        <f>(G10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*G10+C8</f>
-        <v>669616800001</v>
-      </c>
-      <c r="H12" s="40">
-        <f>(H10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*H10+C8</f>
-        <v>785868200001</v>
-      </c>
-      <c r="I12" s="41">
-        <f>(I10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*I10+C8</f>
-        <v>911419600001</v>
-      </c>
-      <c r="J12" s="41">
-        <f>(J10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*J10+C8</f>
-        <v>1046271000001</v>
-      </c>
-      <c r="K12" s="41">
-        <f>(K10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*K10+C8</f>
-        <v>1190422400001</v>
-      </c>
-      <c r="L12" s="41">
-        <f>(L10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*L10+C8</f>
-        <v>1343873800001</v>
-      </c>
-      <c r="M12" s="41">
-        <f>(M10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*M10+C8</f>
-        <v>1506625200001</v>
-      </c>
-      <c r="N12" s="41">
-        <f>(N10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*N10+C8</f>
-        <v>1678676600001</v>
-      </c>
-      <c r="O12" s="41">
-        <f>(O10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*O10+C8</f>
-        <v>1860028000001</v>
-      </c>
-      <c r="P12" s="41">
-        <f>(P10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*P10+C8</f>
-        <v>2050679400001</v>
-      </c>
-      <c r="Q12" s="41">
-        <f>(Q10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*Q10+C8</f>
-        <v>2250630800001</v>
-      </c>
-      <c r="R12" s="41">
-        <f>(R10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*R10+C8</f>
-        <v>2459882200001</v>
-      </c>
-      <c r="S12" s="41">
-        <f>(S10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*S10+C8</f>
-        <v>2678433600001</v>
-      </c>
-      <c r="T12" s="41">
-        <f>(T10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*T10+C8</f>
-        <v>2906285000001</v>
-      </c>
-      <c r="U12" s="41">
-        <f>(U10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*U10+C8</f>
-        <v>3143436400001</v>
-      </c>
-      <c r="V12" s="41">
-        <f>(V10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*V10+C8</f>
-        <v>3389887800001</v>
-      </c>
-      <c r="W12" s="41">
-        <f>(W10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*W10+C8</f>
-        <v>3645639200001</v>
-      </c>
-      <c r="X12" s="41">
-        <f>(X10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*X10+C8</f>
-        <v>3910690600001</v>
-      </c>
-      <c r="Y12" s="41">
-        <f>(Y10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*Y10+C8</f>
-        <v>4185042000001</v>
-      </c>
-      <c r="Z12" s="41">
-        <f>(Z10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*Z10+C8</f>
-        <v>4468693400001</v>
-      </c>
-      <c r="AA12" s="41">
-        <f>(AA10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*AA10+C8</f>
-        <v>4761644800001</v>
-      </c>
-      <c r="AB12" s="41">
-        <f>(AB10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*AB10+C8</f>
-        <v>5063896200001</v>
-      </c>
-      <c r="AC12" s="41">
-        <f>(AC10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*AC10+C8</f>
-        <v>5375447600001</v>
-      </c>
-      <c r="AD12" s="41">
-        <f>(AD10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*AD10+C8</f>
-        <v>5696299000001</v>
-      </c>
-      <c r="AE12" s="41">
-        <f>(AE10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*AE10+C8</f>
-        <v>6026450400001</v>
+      <c r="B12" s="41">
+        <v>23583429</v>
+      </c>
+      <c r="C12" s="29">
+        <v>94166929</v>
+      </c>
+      <c r="D12" s="29">
+        <v>211750429</v>
+      </c>
+      <c r="E12" s="29">
+        <v>376333929</v>
+      </c>
+      <c r="F12" s="29">
+        <v>587917429</v>
+      </c>
+      <c r="G12" s="29">
+        <v>846500929</v>
+      </c>
+      <c r="H12" s="29">
+        <v>1152084429</v>
+      </c>
+      <c r="I12" s="29">
+        <v>1504667929</v>
+      </c>
+      <c r="J12" s="29">
+        <v>1904251429</v>
+      </c>
+      <c r="K12" s="29">
+        <v>2350834929</v>
+      </c>
+      <c r="L12" s="29">
+        <v>2844418429</v>
+      </c>
+      <c r="M12" s="29">
+        <v>3385001929</v>
+      </c>
+      <c r="N12" s="29">
+        <v>3972585429</v>
+      </c>
+      <c r="O12" s="29">
+        <v>4607168929</v>
+      </c>
+      <c r="P12" s="29">
+        <v>5288752429</v>
+      </c>
+      <c r="Q12" s="29">
+        <v>6017335929</v>
+      </c>
+      <c r="R12" s="29">
+        <v>6792919429</v>
+      </c>
+      <c r="S12" s="29">
+        <v>7615502929</v>
+      </c>
+      <c r="T12" s="29">
+        <v>8485086429</v>
+      </c>
+      <c r="U12" s="29">
+        <v>9401669929</v>
+      </c>
+      <c r="V12" s="29">
+        <v>10365253429</v>
+      </c>
+      <c r="W12" s="29">
+        <v>11375836929</v>
+      </c>
+      <c r="X12" s="29">
+        <v>12433420429</v>
+      </c>
+      <c r="Y12" s="29">
+        <v>13538003929</v>
+      </c>
+      <c r="Z12" s="29">
+        <v>14689587429</v>
+      </c>
+      <c r="AA12" s="29">
+        <v>15888170929</v>
+      </c>
+      <c r="AB12" s="29">
+        <v>17133754429</v>
+      </c>
+      <c r="AC12" s="29">
+        <v>18426337929</v>
+      </c>
+      <c r="AD12" s="29">
+        <v>19765921429</v>
+      </c>
+      <c r="AE12" s="29">
+        <v>21152504929</v>
       </c>
     </row>
     <row r="13" spans="1:31" ht="17">
-      <c r="A13" s="12"/>
-      <c r="B13" s="12"/>
-      <c r="C13" s="25"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="25"/>
+      <c r="C13" s="20"/>
+      <c r="H13" s="20"/>
     </row>
     <row r="14" spans="1:31" s="29" customFormat="1">
-      <c r="A14" s="32" t="s">
+      <c r="A14" s="30" t="s">
         <v>2</v>
       </c>
       <c r="B14" s="29">
-        <f>(B10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*B10+H7</f>
-        <v>171514560001</v>
+        <v>14231096</v>
       </c>
       <c r="C14" s="29">
-        <f>(C10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*C10+H7</f>
-        <v>224016640001</v>
+        <v>56712346</v>
       </c>
       <c r="D14" s="29">
-        <f>(D10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*D10+H7</f>
-        <v>283518720001</v>
+        <v>127443596</v>
       </c>
       <c r="E14" s="29">
-        <f>(E10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*E10+H7</f>
-        <v>350020800001</v>
+        <v>226424846</v>
       </c>
       <c r="F14" s="29">
-        <f>(F10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*F10+H7</f>
-        <v>423522880001</v>
+        <v>353656096</v>
       </c>
       <c r="G14" s="29">
-        <f>(G10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*G10+H7</f>
-        <v>504024960001</v>
+        <v>509137346</v>
       </c>
       <c r="H14" s="29">
-        <f>(H10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*H10+H7</f>
-        <v>591527040001</v>
+        <v>692868596</v>
       </c>
       <c r="I14" s="29">
-        <f>(I10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*I10+H7</f>
-        <v>686029120001</v>
+        <v>904849846</v>
       </c>
       <c r="J14" s="29">
-        <f>(J10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*J10+H7</f>
-        <v>787531200001</v>
+        <v>1145081096</v>
       </c>
       <c r="K14" s="29">
-        <f>(K10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*K10+H7</f>
-        <v>896033280001</v>
+        <v>1413562346</v>
       </c>
       <c r="L14" s="29">
-        <f>(L10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*L10+H7</f>
-        <v>1011535360001</v>
+        <v>1710293596</v>
       </c>
       <c r="M14" s="29">
-        <f>(M10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*M10+H7</f>
-        <v>1134037440001</v>
+        <v>2035274846</v>
       </c>
       <c r="N14" s="29">
-        <f>(N10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*N10+H7</f>
-        <v>1263539520001</v>
+        <v>2388506096</v>
       </c>
       <c r="O14" s="29">
-        <f>(O10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*O10+H7</f>
-        <v>1400041600001</v>
+        <v>2769987346</v>
       </c>
       <c r="P14" s="29">
-        <f>(P10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*P10+H7</f>
-        <v>1543543680001</v>
+        <v>3179718596</v>
       </c>
       <c r="Q14" s="29">
-        <f>(Q10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*Q10+H7</f>
-        <v>1694045760001</v>
+        <v>3617699846</v>
       </c>
       <c r="R14" s="29">
-        <f>(R10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*R10+H7</f>
-        <v>1851547840001</v>
+        <v>4083931096</v>
       </c>
       <c r="S14" s="29">
-        <f>(S10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*S10+H7</f>
-        <v>2016049920001</v>
+        <v>4578412346</v>
       </c>
       <c r="T14" s="29">
-        <f>(T10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*T10+H7</f>
-        <v>2187552000001</v>
+        <v>5101143596</v>
       </c>
       <c r="U14" s="29">
-        <f>(U10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*U10+H7</f>
-        <v>2366054080001</v>
+        <v>5652124846</v>
       </c>
       <c r="V14" s="29">
-        <f>(V10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*V10+H7</f>
-        <v>2551556160001</v>
+        <v>6231356096</v>
       </c>
       <c r="W14" s="29">
-        <f>(W10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*W10+H7</f>
-        <v>2744058240001</v>
+        <v>6838837346</v>
       </c>
       <c r="X14" s="29">
-        <f>(X10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*X10+H7</f>
-        <v>2943560320001</v>
+        <v>7474568596</v>
       </c>
       <c r="Y14" s="29">
-        <f>(Y10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*Y10+H7</f>
-        <v>3150062400001</v>
+        <v>8138549846</v>
       </c>
       <c r="Z14" s="29">
-        <f>(Z10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*Z10+H7</f>
-        <v>3363564480001</v>
+        <v>8830781096</v>
       </c>
       <c r="AA14" s="29">
-        <f>(AA10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*AA10+H7</f>
-        <v>3584066560001</v>
+        <v>9551262346</v>
       </c>
       <c r="AB14" s="29">
-        <f>(AB10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*AB10+H7</f>
-        <v>3811568640001</v>
+        <v>10299993596</v>
       </c>
       <c r="AC14" s="29">
-        <f>(AC10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*AC10+H7</f>
-        <v>4046070720001</v>
+        <v>11076974846</v>
       </c>
       <c r="AD14" s="29">
-        <f>(AD10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*AD10+H7</f>
-        <v>4287572800001</v>
+        <v>11882206096</v>
       </c>
       <c r="AE14" s="29">
-        <f>(AE10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*AE10+H7</f>
-        <v>4536074880001</v>
+        <v>12715687346</v>
       </c>
     </row>
     <row r="15" spans="1:31" ht="17">
@@ -5026,7 +4935,7 @@
       <c r="H15" s="25"/>
     </row>
     <row r="16" spans="1:31" ht="18">
-      <c r="D16" s="36" t="s">
+      <c r="D16" s="33" t="s">
         <v>13</v>
       </c>
     </row>
@@ -5047,7 +4956,7 @@
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H38" sqref="H38"/>
+      <selection pane="bottomLeft" activeCell="A12" sqref="A12:XFD14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5225,98 +5134,98 @@
       <c r="G9" s="12"/>
       <c r="H9" s="27"/>
     </row>
-    <row r="10" spans="1:31" s="43" customFormat="1" ht="17">
-      <c r="A10" s="42" t="s">
+    <row r="10" spans="1:31" s="38" customFormat="1" ht="17">
+      <c r="A10" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="43">
+      <c r="B10" s="38">
         <v>40000</v>
       </c>
-      <c r="C10" s="43">
+      <c r="C10" s="38">
         <v>45000</v>
       </c>
-      <c r="D10" s="43">
+      <c r="D10" s="38">
         <v>50000</v>
       </c>
-      <c r="E10" s="43">
+      <c r="E10" s="38">
         <v>55000</v>
       </c>
-      <c r="F10" s="43">
+      <c r="F10" s="38">
         <v>60000</v>
       </c>
-      <c r="G10" s="43">
+      <c r="G10" s="38">
         <v>65000</v>
       </c>
-      <c r="H10" s="43">
+      <c r="H10" s="38">
         <v>70000</v>
       </c>
-      <c r="I10" s="43">
+      <c r="I10" s="38">
         <v>75000</v>
       </c>
-      <c r="J10" s="43">
+      <c r="J10" s="38">
         <v>80000</v>
       </c>
-      <c r="K10" s="43">
+      <c r="K10" s="38">
         <v>85000</v>
       </c>
-      <c r="L10" s="43">
+      <c r="L10" s="38">
         <v>90000</v>
       </c>
-      <c r="M10" s="43">
+      <c r="M10" s="38">
         <v>95000</v>
       </c>
-      <c r="N10" s="43">
+      <c r="N10" s="38">
         <v>100000</v>
       </c>
-      <c r="O10" s="43">
+      <c r="O10" s="38">
         <v>105000</v>
       </c>
-      <c r="P10" s="43">
+      <c r="P10" s="38">
         <v>110000</v>
       </c>
-      <c r="Q10" s="43">
+      <c r="Q10" s="38">
         <v>115000</v>
       </c>
-      <c r="R10" s="43">
+      <c r="R10" s="38">
         <v>120000</v>
       </c>
-      <c r="S10" s="43">
+      <c r="S10" s="38">
         <v>125000</v>
       </c>
-      <c r="T10" s="43">
+      <c r="T10" s="38">
         <v>130000</v>
       </c>
-      <c r="U10" s="43">
+      <c r="U10" s="38">
         <v>135000</v>
       </c>
-      <c r="V10" s="43">
+      <c r="V10" s="38">
         <v>140000</v>
       </c>
-      <c r="W10" s="43">
+      <c r="W10" s="38">
         <v>145000</v>
       </c>
-      <c r="X10" s="43">
+      <c r="X10" s="38">
         <v>150000</v>
       </c>
-      <c r="Y10" s="43">
+      <c r="Y10" s="38">
         <v>155000</v>
       </c>
-      <c r="Z10" s="43">
+      <c r="Z10" s="38">
         <v>160000</v>
       </c>
-      <c r="AA10" s="43">
+      <c r="AA10" s="38">
         <v>165000</v>
       </c>
-      <c r="AB10" s="43">
+      <c r="AB10" s="38">
         <v>170000</v>
       </c>
-      <c r="AC10" s="43">
+      <c r="AC10" s="38">
         <v>175000</v>
       </c>
-      <c r="AD10" s="43">
+      <c r="AD10" s="38">
         <v>180000</v>
       </c>
-      <c r="AE10" s="43">
+      <c r="AE10" s="38">
         <v>185000</v>
       </c>
     </row>
@@ -5330,264 +5239,198 @@
       <c r="G11" s="12"/>
       <c r="H11" s="27"/>
     </row>
-    <row r="12" spans="1:31" s="30" customFormat="1">
-      <c r="A12" s="32" t="s">
+    <row r="12" spans="1:31" s="29" customFormat="1">
+      <c r="A12" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="30">
-        <f>(B10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*B10+C8</f>
-        <v>337610960008</v>
-      </c>
-      <c r="C12" s="30">
-        <f>(C10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*C10+C8</f>
-        <v>427287330008</v>
-      </c>
-      <c r="D12" s="30">
-        <f>(D10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*D10+C8</f>
-        <v>527513700008</v>
-      </c>
-      <c r="E12" s="30">
-        <f>(E10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*E10+C8</f>
-        <v>638290070008</v>
-      </c>
-      <c r="F12" s="30">
-        <f>(F10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*F10+C8</f>
-        <v>759616440008</v>
-      </c>
-      <c r="G12" s="30">
-        <f>(G10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*G10+C8</f>
-        <v>891492810008</v>
-      </c>
-      <c r="H12" s="30">
-        <f>(H10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*H10+C8</f>
-        <v>1033919180008</v>
-      </c>
-      <c r="I12" s="30">
-        <f>(I10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*I10+C8</f>
-        <v>1186895550008</v>
-      </c>
-      <c r="J12" s="30">
-        <f>(J10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*J10+C8</f>
-        <v>1350421920008</v>
-      </c>
-      <c r="K12" s="30">
-        <f>(K10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*K10+C8</f>
-        <v>1524498290008</v>
-      </c>
-      <c r="L12" s="30">
-        <f>(L10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*L10+C8</f>
-        <v>1709124660008</v>
-      </c>
-      <c r="M12" s="30">
-        <f>(M10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*M10+C8</f>
-        <v>1904301030008</v>
-      </c>
-      <c r="N12" s="30">
-        <f>(N10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*N10+C8</f>
-        <v>2110027400008</v>
-      </c>
-      <c r="O12" s="30">
-        <f>(O10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*O10+C8</f>
-        <v>2326303770008</v>
-      </c>
-      <c r="P12" s="30">
-        <f>(P10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*P10+C8</f>
-        <v>2553130140008</v>
-      </c>
-      <c r="Q12" s="30">
-        <f>(Q10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*Q10+C8</f>
-        <v>2790506510008</v>
-      </c>
-      <c r="R12" s="30">
-        <f>(R10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*R10+C8</f>
-        <v>3038432880008</v>
-      </c>
-      <c r="S12" s="30">
-        <f>(S10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*S10+C8</f>
-        <v>3296909250008</v>
-      </c>
-      <c r="T12" s="30">
-        <f>(T10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*T10+C8</f>
-        <v>3565935620008</v>
-      </c>
-      <c r="U12" s="30">
-        <f>(U10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*U10+C8</f>
-        <v>3845511990008</v>
-      </c>
-      <c r="V12" s="30">
-        <f>(V10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*V10+C8</f>
-        <v>4135638360008</v>
-      </c>
-      <c r="W12" s="30">
-        <f>(W10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*W10+C8</f>
-        <v>4436314730008</v>
-      </c>
-      <c r="X12" s="30">
-        <f>(X10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*X10+C8</f>
-        <v>4747541100008</v>
-      </c>
-      <c r="Y12" s="30">
-        <f>(Y10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*Y10+C8</f>
-        <v>5069317470008</v>
-      </c>
-      <c r="Z12" s="30">
-        <f>(Z10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*Z10+C8</f>
-        <v>5401643840008</v>
-      </c>
-      <c r="AA12" s="30">
-        <f>(AA10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*AA10+C8</f>
-        <v>5744520210008</v>
-      </c>
-      <c r="AB12" s="30">
-        <f>(AB10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*AB10+C8</f>
-        <v>6097946580008</v>
-      </c>
-      <c r="AC12" s="30">
-        <f>(AC10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*AC10+C8</f>
-        <v>6461922950008</v>
-      </c>
-      <c r="AD12" s="30">
-        <f>(AD10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*AD10+C8</f>
-        <v>6836449320008</v>
-      </c>
-      <c r="AE12" s="30">
-        <f>(AE10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*AE10+C8</f>
-        <v>7221525690008</v>
-      </c>
-    </row>
-    <row r="13" spans="1:31">
-      <c r="A13" s="12"/>
-      <c r="B13" s="12"/>
-      <c r="C13" s="27"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="27"/>
+      <c r="B12" s="41">
+        <v>23583429</v>
+      </c>
+      <c r="C12" s="29">
+        <v>94166929</v>
+      </c>
+      <c r="D12" s="29">
+        <v>211750429</v>
+      </c>
+      <c r="E12" s="29">
+        <v>376333929</v>
+      </c>
+      <c r="F12" s="29">
+        <v>587917429</v>
+      </c>
+      <c r="G12" s="29">
+        <v>846500929</v>
+      </c>
+      <c r="H12" s="29">
+        <v>1152084429</v>
+      </c>
+      <c r="I12" s="29">
+        <v>1504667929</v>
+      </c>
+      <c r="J12" s="29">
+        <v>1904251429</v>
+      </c>
+      <c r="K12" s="29">
+        <v>2350834929</v>
+      </c>
+      <c r="L12" s="29">
+        <v>2844418429</v>
+      </c>
+      <c r="M12" s="29">
+        <v>3385001929</v>
+      </c>
+      <c r="N12" s="29">
+        <v>3972585429</v>
+      </c>
+      <c r="O12" s="29">
+        <v>4607168929</v>
+      </c>
+      <c r="P12" s="29">
+        <v>5288752429</v>
+      </c>
+      <c r="Q12" s="29">
+        <v>6017335929</v>
+      </c>
+      <c r="R12" s="29">
+        <v>6792919429</v>
+      </c>
+      <c r="S12" s="29">
+        <v>7615502929</v>
+      </c>
+      <c r="T12" s="29">
+        <v>8485086429</v>
+      </c>
+      <c r="U12" s="29">
+        <v>9401669929</v>
+      </c>
+      <c r="V12" s="29">
+        <v>10365253429</v>
+      </c>
+      <c r="W12" s="29">
+        <v>11375836929</v>
+      </c>
+      <c r="X12" s="29">
+        <v>12433420429</v>
+      </c>
+      <c r="Y12" s="29">
+        <v>13538003929</v>
+      </c>
+      <c r="Z12" s="29">
+        <v>14689587429</v>
+      </c>
+      <c r="AA12" s="29">
+        <v>15888170929</v>
+      </c>
+      <c r="AB12" s="29">
+        <v>17133754429</v>
+      </c>
+      <c r="AC12" s="29">
+        <v>18426337929</v>
+      </c>
+      <c r="AD12" s="29">
+        <v>19765921429</v>
+      </c>
+      <c r="AE12" s="29">
+        <v>21152504929</v>
+      </c>
+    </row>
+    <row r="13" spans="1:31" ht="17">
+      <c r="C13" s="20"/>
+      <c r="H13" s="20"/>
     </row>
     <row r="14" spans="1:31" s="29" customFormat="1">
-      <c r="A14" s="32" t="s">
+      <c r="A14" s="30" t="s">
         <v>2</v>
       </c>
       <c r="B14" s="29">
-        <f>(B10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*B10+H7</f>
-        <v>216012360008</v>
+        <v>14231096</v>
       </c>
       <c r="C14" s="29">
-        <f>(C10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*C10+H7</f>
-        <v>273388905008</v>
+        <v>56712346</v>
       </c>
       <c r="D14" s="29">
-        <f>(D10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*D10+H7</f>
-        <v>337515450008</v>
+        <v>127443596</v>
       </c>
       <c r="E14" s="29">
-        <f>(E10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*E10+H7</f>
-        <v>408391995008</v>
+        <v>226424846</v>
       </c>
       <c r="F14" s="29">
-        <f>(F10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*F10+H7</f>
-        <v>486018540008</v>
+        <v>353656096</v>
       </c>
       <c r="G14" s="29">
-        <f>(G10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*G10+H7</f>
-        <v>570395085008</v>
+        <v>509137346</v>
       </c>
       <c r="H14" s="29">
-        <f>(H10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*H10+H7</f>
-        <v>661521630008</v>
+        <v>692868596</v>
       </c>
       <c r="I14" s="29">
-        <f>(I10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*I10+H7</f>
-        <v>759398175008</v>
+        <v>904849846</v>
       </c>
       <c r="J14" s="29">
-        <f>(J10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*J10+H7</f>
-        <v>864024720008</v>
+        <v>1145081096</v>
       </c>
       <c r="K14" s="29">
-        <f>(K10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*K10+H7</f>
-        <v>975401265008</v>
+        <v>1413562346</v>
       </c>
       <c r="L14" s="29">
-        <f>(L10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*L10+H7</f>
-        <v>1093527810008</v>
+        <v>1710293596</v>
       </c>
       <c r="M14" s="29">
-        <f>(M10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*M10+H7</f>
-        <v>1218404355008</v>
+        <v>2035274846</v>
       </c>
       <c r="N14" s="29">
-        <f>(N10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*N10+H7</f>
-        <v>1350030900008</v>
+        <v>2388506096</v>
       </c>
       <c r="O14" s="29">
-        <f>(O10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*O10+H7</f>
-        <v>1488407445008</v>
+        <v>2769987346</v>
       </c>
       <c r="P14" s="29">
-        <f>(P10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*P10+H7</f>
-        <v>1633533990008</v>
+        <v>3179718596</v>
       </c>
       <c r="Q14" s="29">
-        <f>(Q10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*Q10+H7</f>
-        <v>1785410535008</v>
+        <v>3617699846</v>
       </c>
       <c r="R14" s="29">
-        <f>(R10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*R10+H7</f>
-        <v>1944037080008</v>
+        <v>4083931096</v>
       </c>
       <c r="S14" s="29">
-        <f>(S10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*S10+H7</f>
-        <v>2109413625008</v>
+        <v>4578412346</v>
       </c>
       <c r="T14" s="29">
-        <f>(T10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*T10+H7</f>
-        <v>2281540170008</v>
+        <v>5101143596</v>
       </c>
       <c r="U14" s="29">
-        <f>(U10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*U10+H7</f>
-        <v>2460416715008</v>
+        <v>5652124846</v>
       </c>
       <c r="V14" s="29">
-        <f>(V10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*V10+H7</f>
-        <v>2646043260008</v>
+        <v>6231356096</v>
       </c>
       <c r="W14" s="29">
-        <f>(W10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*W10+H7</f>
-        <v>2838419805008</v>
+        <v>6838837346</v>
       </c>
       <c r="X14" s="29">
-        <f>(X10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*X10+H7</f>
-        <v>3037546350008</v>
+        <v>7474568596</v>
       </c>
       <c r="Y14" s="29">
-        <f>(Y10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*Y10+H7</f>
-        <v>3243422895008</v>
+        <v>8138549846</v>
       </c>
       <c r="Z14" s="29">
-        <f>(Z10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*Z10+H7</f>
-        <v>3456049440008</v>
+        <v>8830781096</v>
       </c>
       <c r="AA14" s="29">
-        <f>(AA10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*AA10+H7</f>
-        <v>3675425985008</v>
+        <v>9551262346</v>
       </c>
       <c r="AB14" s="29">
-        <f>(AB10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*AB10+H7</f>
-        <v>3901552530008</v>
+        <v>10299993596</v>
       </c>
       <c r="AC14" s="29">
-        <f>(AC10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*AC10+H7</f>
-        <v>4134429075008</v>
+        <v>11076974846</v>
       </c>
       <c r="AD14" s="29">
-        <f>(AD10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*AD10+H7</f>
-        <v>4374055620008</v>
+        <v>11882206096</v>
       </c>
       <c r="AE14" s="29">
-        <f>(AE10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*AE10+H7</f>
-        <v>4620432165008</v>
+        <v>12715687346</v>
       </c>
     </row>
     <row r="15" spans="1:31">
@@ -5601,7 +5444,7 @@
       <c r="H15" s="27"/>
     </row>
     <row r="16" spans="1:31" ht="18">
-      <c r="D16" s="36" t="s">
+      <c r="D16" s="33" t="s">
         <v>13</v>
       </c>
     </row>
@@ -5623,7 +5466,7 @@
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
+      <selection pane="bottomLeft" activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5797,98 +5640,98 @@
       <c r="G9" s="12"/>
       <c r="H9" s="17"/>
     </row>
-    <row r="10" spans="1:31" s="45" customFormat="1" ht="17">
-      <c r="A10" s="44" t="s">
+    <row r="10" spans="1:31" s="40" customFormat="1" ht="17">
+      <c r="A10" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="45">
+      <c r="B10" s="40">
         <v>70000</v>
       </c>
-      <c r="C10" s="44">
+      <c r="C10" s="39">
         <v>75000</v>
       </c>
-      <c r="D10" s="45">
+      <c r="D10" s="40">
         <v>80000</v>
       </c>
-      <c r="E10" s="44">
+      <c r="E10" s="39">
         <v>85000</v>
       </c>
-      <c r="F10" s="45">
+      <c r="F10" s="40">
         <v>90000</v>
       </c>
-      <c r="G10" s="44">
+      <c r="G10" s="39">
         <v>95000</v>
       </c>
-      <c r="H10" s="45">
+      <c r="H10" s="40">
         <v>100000</v>
       </c>
-      <c r="I10" s="44">
+      <c r="I10" s="39">
         <v>105000</v>
       </c>
-      <c r="J10" s="45">
+      <c r="J10" s="40">
         <v>110000</v>
       </c>
-      <c r="K10" s="44">
+      <c r="K10" s="39">
         <v>115000</v>
       </c>
-      <c r="L10" s="45">
+      <c r="L10" s="40">
         <v>120000</v>
       </c>
-      <c r="M10" s="44">
+      <c r="M10" s="39">
         <v>125000</v>
       </c>
-      <c r="N10" s="45">
+      <c r="N10" s="40">
         <v>130000</v>
       </c>
-      <c r="O10" s="44">
+      <c r="O10" s="39">
         <v>135000</v>
       </c>
-      <c r="P10" s="45">
+      <c r="P10" s="40">
         <v>140000</v>
       </c>
-      <c r="Q10" s="44">
+      <c r="Q10" s="39">
         <v>145000</v>
       </c>
-      <c r="R10" s="45">
+      <c r="R10" s="40">
         <v>150000</v>
       </c>
-      <c r="S10" s="44">
+      <c r="S10" s="39">
         <v>155000</v>
       </c>
-      <c r="T10" s="45">
+      <c r="T10" s="40">
         <v>160000</v>
       </c>
-      <c r="U10" s="44">
+      <c r="U10" s="39">
         <v>165000</v>
       </c>
-      <c r="V10" s="45">
+      <c r="V10" s="40">
         <v>170000</v>
       </c>
-      <c r="W10" s="44">
+      <c r="W10" s="39">
         <v>175000</v>
       </c>
-      <c r="X10" s="45">
+      <c r="X10" s="40">
         <v>180000</v>
       </c>
-      <c r="Y10" s="44">
+      <c r="Y10" s="39">
         <v>185000</v>
       </c>
-      <c r="Z10" s="45">
+      <c r="Z10" s="40">
         <v>190000</v>
       </c>
-      <c r="AA10" s="44">
+      <c r="AA10" s="39">
         <v>195000</v>
       </c>
-      <c r="AB10" s="45">
+      <c r="AB10" s="40">
         <v>200000</v>
       </c>
-      <c r="AC10" s="44">
+      <c r="AC10" s="39">
         <v>205000</v>
       </c>
-      <c r="AD10" s="45">
+      <c r="AD10" s="40">
         <v>210000</v>
       </c>
-      <c r="AE10" s="44">
+      <c r="AE10" s="39">
         <v>215000</v>
       </c>
     </row>
@@ -5902,264 +5745,198 @@
       <c r="G11" s="12"/>
       <c r="H11" s="17"/>
     </row>
-    <row r="12" spans="1:31" s="30" customFormat="1">
-      <c r="A12" s="31" t="s">
+    <row r="12" spans="1:31" s="29" customFormat="1">
+      <c r="A12" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="30">
-        <f>(B10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*B10+C8</f>
-        <v>774215330006</v>
-      </c>
-      <c r="C12" s="30">
-        <f>(C10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*C10+C8</f>
-        <v>888766425006</v>
-      </c>
-      <c r="D12" s="30">
-        <f>(D10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*D10+C8</f>
-        <v>1011217520006</v>
-      </c>
-      <c r="E12" s="30">
-        <f>(E10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*E10+C8</f>
-        <v>1141568615006</v>
-      </c>
-      <c r="F12" s="30">
-        <f>(F10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*F10+C8</f>
-        <v>1279819710006</v>
-      </c>
-      <c r="G12" s="30">
-        <f>(G10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*G10+C8</f>
-        <v>1425970805006</v>
-      </c>
-      <c r="H12" s="30">
-        <f>(H10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*H10+C8</f>
-        <v>1580021900006</v>
-      </c>
-      <c r="I12" s="30">
-        <f>(I10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*I10+C8</f>
-        <v>1741972995006</v>
-      </c>
-      <c r="J12" s="30">
-        <f>(J10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*J10+C8</f>
-        <v>1911824090006</v>
-      </c>
-      <c r="K12" s="30">
-        <f>(K10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*K10+C8</f>
-        <v>2089575185006</v>
-      </c>
-      <c r="L12" s="30">
-        <f>(L10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*L10+C8</f>
-        <v>2275226280006</v>
-      </c>
-      <c r="M12" s="30">
-        <f>(M10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*M10+C8</f>
-        <v>2468777375006</v>
-      </c>
-      <c r="N12" s="30">
-        <f>(N10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*N10+C8</f>
-        <v>2670228470006</v>
-      </c>
-      <c r="O12" s="30">
-        <f>(O10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*O10+C8</f>
-        <v>2879579565006</v>
-      </c>
-      <c r="P12" s="30">
-        <f>(P10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*P10+C8</f>
-        <v>3096830660006</v>
-      </c>
-      <c r="Q12" s="30">
-        <f>(Q10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*Q10+C8</f>
-        <v>3321981755006</v>
-      </c>
-      <c r="R12" s="30">
-        <f>(R10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*R10+C8</f>
-        <v>3555032850006</v>
-      </c>
-      <c r="S12" s="30">
-        <f>(S10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*S10+C8</f>
-        <v>3795983945006</v>
-      </c>
-      <c r="T12" s="30">
-        <f>(T10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*T10+C8</f>
-        <v>4044835040006</v>
-      </c>
-      <c r="U12" s="30">
-        <f>(U10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*U10+C8</f>
-        <v>4301586135006</v>
-      </c>
-      <c r="V12" s="30">
-        <f>(V10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*V10+C8</f>
-        <v>4566237230006</v>
-      </c>
-      <c r="W12" s="30">
-        <f>(W10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*W10+C8</f>
-        <v>4838788325006</v>
-      </c>
-      <c r="X12" s="30">
-        <f>(X10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*X10+C8</f>
-        <v>5119239420006</v>
-      </c>
-      <c r="Y12" s="30">
-        <f>(Y10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*Y10+C8</f>
-        <v>5407590515006</v>
-      </c>
-      <c r="Z12" s="30">
-        <f>(Z10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*Z10+C8</f>
-        <v>5703841610006</v>
-      </c>
-      <c r="AA12" s="30">
-        <f>(AA10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*AA10+C8</f>
-        <v>6007992705006</v>
-      </c>
-      <c r="AB12" s="30">
-        <f>(AB10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*AB10+C8</f>
-        <v>6320043800006</v>
-      </c>
-      <c r="AC12" s="30">
-        <f>(AC10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*AC10+C8</f>
-        <v>6639994895006</v>
-      </c>
-      <c r="AD12" s="30">
-        <f>(AD10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*AD10+C8</f>
-        <v>6967845990006</v>
-      </c>
-      <c r="AE12" s="30">
-        <f>(AE10^2)*(2*C5+2*C7+2*C4+C3)+(2*C3+4*C6+5*C4)*AE10+C8</f>
-        <v>7303597085006</v>
-      </c>
-    </row>
-    <row r="13" spans="1:31">
-      <c r="A13" s="12"/>
-      <c r="B13" s="12"/>
-      <c r="C13" s="17"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="17"/>
+      <c r="B12" s="41">
+        <v>23583429</v>
+      </c>
+      <c r="C12" s="29">
+        <v>94166929</v>
+      </c>
+      <c r="D12" s="29">
+        <v>211750429</v>
+      </c>
+      <c r="E12" s="29">
+        <v>376333929</v>
+      </c>
+      <c r="F12" s="29">
+        <v>587917429</v>
+      </c>
+      <c r="G12" s="29">
+        <v>846500929</v>
+      </c>
+      <c r="H12" s="29">
+        <v>1152084429</v>
+      </c>
+      <c r="I12" s="29">
+        <v>1504667929</v>
+      </c>
+      <c r="J12" s="29">
+        <v>1904251429</v>
+      </c>
+      <c r="K12" s="29">
+        <v>2350834929</v>
+      </c>
+      <c r="L12" s="29">
+        <v>2844418429</v>
+      </c>
+      <c r="M12" s="29">
+        <v>3385001929</v>
+      </c>
+      <c r="N12" s="29">
+        <v>3972585429</v>
+      </c>
+      <c r="O12" s="29">
+        <v>4607168929</v>
+      </c>
+      <c r="P12" s="29">
+        <v>5288752429</v>
+      </c>
+      <c r="Q12" s="29">
+        <v>6017335929</v>
+      </c>
+      <c r="R12" s="29">
+        <v>6792919429</v>
+      </c>
+      <c r="S12" s="29">
+        <v>7615502929</v>
+      </c>
+      <c r="T12" s="29">
+        <v>8485086429</v>
+      </c>
+      <c r="U12" s="29">
+        <v>9401669929</v>
+      </c>
+      <c r="V12" s="29">
+        <v>10365253429</v>
+      </c>
+      <c r="W12" s="29">
+        <v>11375836929</v>
+      </c>
+      <c r="X12" s="29">
+        <v>12433420429</v>
+      </c>
+      <c r="Y12" s="29">
+        <v>13538003929</v>
+      </c>
+      <c r="Z12" s="29">
+        <v>14689587429</v>
+      </c>
+      <c r="AA12" s="29">
+        <v>15888170929</v>
+      </c>
+      <c r="AB12" s="29">
+        <v>17133754429</v>
+      </c>
+      <c r="AC12" s="29">
+        <v>18426337929</v>
+      </c>
+      <c r="AD12" s="29">
+        <v>19765921429</v>
+      </c>
+      <c r="AE12" s="29">
+        <v>21152504929</v>
+      </c>
+    </row>
+    <row r="13" spans="1:31" ht="17">
+      <c r="C13" s="20"/>
+      <c r="H13" s="20"/>
     </row>
     <row r="14" spans="1:31" s="29" customFormat="1">
-      <c r="A14" s="32" t="s">
+      <c r="A14" s="30" t="s">
         <v>2</v>
       </c>
       <c r="B14" s="29">
-        <f>(B10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*B10+H7</f>
-        <v>504721210006</v>
+        <v>14231096</v>
       </c>
       <c r="C14" s="29">
-        <f>(C10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*C10+H7</f>
-        <v>579397725006</v>
+        <v>56712346</v>
       </c>
       <c r="D14" s="29">
-        <f>(D10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*D10+H7</f>
-        <v>659224240006</v>
+        <v>127443596</v>
       </c>
       <c r="E14" s="29">
-        <f>(E10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*E10+H7</f>
-        <v>744200755006</v>
+        <v>226424846</v>
       </c>
       <c r="F14" s="29">
-        <f>(F10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*F10+H7</f>
-        <v>834327270006</v>
+        <v>353656096</v>
       </c>
       <c r="G14" s="29">
-        <f>(G10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*G10+H7</f>
-        <v>929603785006</v>
+        <v>509137346</v>
       </c>
       <c r="H14" s="29">
-        <f>(H10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*H10+H7</f>
-        <v>1030030300006</v>
+        <v>692868596</v>
       </c>
       <c r="I14" s="29">
-        <f>(I10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*I10+H7</f>
-        <v>1135606815006</v>
+        <v>904849846</v>
       </c>
       <c r="J14" s="29">
-        <f>(J10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*J10+H7</f>
-        <v>1246333330006</v>
+        <v>1145081096</v>
       </c>
       <c r="K14" s="29">
-        <f>(K10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*K10+H7</f>
-        <v>1362209845006</v>
+        <v>1413562346</v>
       </c>
       <c r="L14" s="29">
-        <f>(L10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*L10+H7</f>
-        <v>1483236360006</v>
+        <v>1710293596</v>
       </c>
       <c r="M14" s="29">
-        <f>(M10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*M10+H7</f>
-        <v>1609412875006</v>
+        <v>2035274846</v>
       </c>
       <c r="N14" s="29">
-        <f>(N10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*N10+H7</f>
-        <v>1740739390006</v>
+        <v>2388506096</v>
       </c>
       <c r="O14" s="29">
-        <f>(O10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*O10+H7</f>
-        <v>1877215905006</v>
+        <v>2769987346</v>
       </c>
       <c r="P14" s="29">
-        <f>(P10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*P10+H7</f>
-        <v>2018842420006</v>
+        <v>3179718596</v>
       </c>
       <c r="Q14" s="29">
-        <f>(Q10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*Q10+H7</f>
-        <v>2165618935006</v>
+        <v>3617699846</v>
       </c>
       <c r="R14" s="29">
-        <f>(R10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*R10+H7</f>
-        <v>2317545450006</v>
+        <v>4083931096</v>
       </c>
       <c r="S14" s="29">
-        <f>(S10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*S10+H7</f>
-        <v>2474621965006</v>
+        <v>4578412346</v>
       </c>
       <c r="T14" s="29">
-        <f>(T10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*T10+H7</f>
-        <v>2636848480006</v>
+        <v>5101143596</v>
       </c>
       <c r="U14" s="29">
-        <f>(U10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*U10+H7</f>
-        <v>2804224995006</v>
+        <v>5652124846</v>
       </c>
       <c r="V14" s="29">
-        <f>(V10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*V10+H7</f>
-        <v>2976751510006</v>
+        <v>6231356096</v>
       </c>
       <c r="W14" s="29">
-        <f>(W10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*W10+H7</f>
-        <v>3154428025006</v>
+        <v>6838837346</v>
       </c>
       <c r="X14" s="29">
-        <f>(X10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*X10+H7</f>
-        <v>3337254540006</v>
+        <v>7474568596</v>
       </c>
       <c r="Y14" s="29">
-        <f>(Y10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*Y10+H7</f>
-        <v>3525231055006</v>
+        <v>8138549846</v>
       </c>
       <c r="Z14" s="29">
-        <f>(Z10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*Z10+H7</f>
-        <v>3718357570006</v>
+        <v>8830781096</v>
       </c>
       <c r="AA14" s="29">
-        <f>(AA10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*AA10+H7</f>
-        <v>3916634085006</v>
+        <v>9551262346</v>
       </c>
       <c r="AB14" s="29">
-        <f>(AB10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*AB10+H7</f>
-        <v>4120060600006</v>
+        <v>10299993596</v>
       </c>
       <c r="AC14" s="29">
-        <f>(AC10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*AC10+H7</f>
-        <v>4328637115006</v>
+        <v>11076974846</v>
       </c>
       <c r="AD14" s="29">
-        <f>(AD10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*AD10+H7</f>
-        <v>4542363630006</v>
+        <v>11882206096</v>
       </c>
       <c r="AE14" s="29">
-        <f>(AE10^2)*(2*H4+H5+H3)+(5*H3+H6+5*H4+H7)*AE10+H7</f>
-        <v>4761240145006</v>
+        <v>12715687346</v>
       </c>
     </row>
     <row r="15" spans="1:31">
@@ -6173,7 +5950,7 @@
       <c r="H15" s="17"/>
     </row>
     <row r="16" spans="1:31" ht="18">
-      <c r="E16" s="34" t="s">
+      <c r="E16" s="31" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>